<commit_message>
updated bom with revision numbers
</commit_message>
<xml_diff>
--- a/export/SM_BOM.xlsx
+++ b/export/SM_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="69">
   <si>
     <t>Item #</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>TBD, assume black</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>1.0</t>
   </si>
 </sst>
 </file>
@@ -265,12 +271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,6 +279,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:O49"/>
+  <dimension ref="C1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,187 +598,194 @@
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="12" width="18.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="1" customWidth="1"/>
-    <col min="14" max="14" width="61" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="13" width="18.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16" style="1" customWidth="1"/>
+    <col min="15" max="15" width="61" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-    </row>
-    <row r="21" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+    </row>
+    <row r="21" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I28" s="5" t="s">
+    <row r="24" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="J28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5" t="s">
+      <c r="K28" s="9"/>
+      <c r="L28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M28" s="9"/>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,34 +799,37 @@
         <v>22</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" s="4">
         <v>1</v>
       </c>
@@ -826,37 +842,40 @@
       <c r="F30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I30" s="3">
+      <c r="J30" s="3">
         <v>194.48</v>
       </c>
-      <c r="J30" s="3">
+      <c r="K30" s="3">
         <v>294.48</v>
       </c>
-      <c r="K30" s="7">
-        <f>I30/25.4</f>
+      <c r="L30" s="5">
+        <f>J30/25.4</f>
         <v>7.656692913385827</v>
       </c>
-      <c r="L30" s="7">
-        <f>J30/25.4</f>
+      <c r="M30" s="5">
+        <f>K30/25.4</f>
         <v>11.593700787401577</v>
       </c>
-      <c r="M30" s="8" t="s">
+      <c r="N30" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>21</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C31" s="4">
         <v>2</v>
       </c>
@@ -869,37 +888,40 @@
       <c r="F31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I31" s="3">
+      <c r="J31" s="3">
         <v>464.48</v>
       </c>
-      <c r="J31" s="3">
+      <c r="K31" s="3">
         <v>206.72</v>
       </c>
-      <c r="K31" s="7">
-        <f t="shared" ref="K31:L42" si="0">I31/25.4</f>
+      <c r="L31" s="5">
+        <f t="shared" ref="L31:M42" si="0">J31/25.4</f>
         <v>18.286614173228347</v>
       </c>
-      <c r="L31" s="7">
+      <c r="M31" s="5">
         <f t="shared" si="0"/>
         <v>8.1385826771653544</v>
       </c>
-      <c r="M31" s="8" t="s">
+      <c r="N31" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C32" s="4">
         <v>3</v>
       </c>
@@ -912,37 +934,40 @@
       <c r="F32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I32" s="3">
+      <c r="J32" s="3">
         <v>407.66</v>
       </c>
-      <c r="J32" s="3">
+      <c r="K32" s="3">
         <v>432.26</v>
       </c>
-      <c r="K32" s="7">
+      <c r="L32" s="5">
         <f t="shared" si="0"/>
         <v>16.049606299212602</v>
       </c>
-      <c r="L32" s="7">
+      <c r="M32" s="5">
         <f t="shared" si="0"/>
         <v>17.018110236220473</v>
       </c>
-      <c r="M32" s="8" t="s">
+      <c r="N32" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C33" s="4">
         <v>4</v>
       </c>
@@ -955,37 +980,40 @@
       <c r="F33" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I33" s="3">
+      <c r="J33" s="3">
         <v>407.66</v>
       </c>
-      <c r="J33" s="3">
+      <c r="K33" s="3">
         <v>432.26</v>
       </c>
-      <c r="K33" s="7">
+      <c r="L33" s="5">
         <f t="shared" si="0"/>
         <v>16.049606299212602</v>
       </c>
-      <c r="L33" s="7">
+      <c r="M33" s="5">
         <f t="shared" si="0"/>
         <v>17.018110236220473</v>
       </c>
-      <c r="M33" s="8" t="s">
+      <c r="N33" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="P33" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C34" s="4">
         <v>5</v>
       </c>
@@ -998,37 +1026,40 @@
       <c r="F34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I34" s="3">
+      <c r="J34" s="3">
         <v>704.42</v>
       </c>
-      <c r="J34" s="3">
+      <c r="K34" s="3">
         <v>435.86</v>
       </c>
-      <c r="K34" s="7">
+      <c r="L34" s="5">
         <f t="shared" si="0"/>
         <v>27.73307086614173</v>
       </c>
-      <c r="L34" s="7">
+      <c r="M34" s="5">
         <f t="shared" si="0"/>
         <v>17.159842519685039</v>
       </c>
-      <c r="M34" s="8" t="s">
+      <c r="N34" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="O34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C35" s="4">
         <v>6</v>
       </c>
@@ -1041,37 +1072,40 @@
       <c r="F35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I35" s="3">
-        <v>323.14</v>
       </c>
       <c r="J35" s="3">
         <v>323.14</v>
       </c>
-      <c r="K35" s="7">
+      <c r="K35" s="3">
+        <v>323.14</v>
+      </c>
+      <c r="L35" s="5">
         <f t="shared" si="0"/>
         <v>12.722047244094489</v>
       </c>
-      <c r="L35" s="7">
+      <c r="M35" s="5">
         <f t="shared" si="0"/>
         <v>12.722047244094489</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="N35" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="3:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="4">
         <v>7</v>
       </c>
@@ -1084,37 +1118,40 @@
       <c r="F36" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I36" s="3">
+      <c r="J36" s="3">
         <v>251</v>
       </c>
-      <c r="J36" s="3">
+      <c r="K36" s="3">
         <v>295.10000000000002</v>
       </c>
-      <c r="K36" s="7">
+      <c r="L36" s="5">
         <f t="shared" si="0"/>
         <v>9.8818897637795278</v>
       </c>
-      <c r="L36" s="7">
+      <c r="M36" s="5">
         <f t="shared" si="0"/>
         <v>11.618110236220474</v>
       </c>
-      <c r="M36" s="8" t="s">
+      <c r="N36" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="P36" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C37" s="4">
         <v>8</v>
       </c>
@@ -1127,37 +1164,40 @@
       <c r="F37" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H37" t="s">
         <v>14</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I37" s="3">
+      <c r="J37" s="3">
         <v>350</v>
       </c>
-      <c r="J37" s="3">
+      <c r="K37" s="3">
         <v>269.48</v>
       </c>
-      <c r="K37" s="7">
+      <c r="L37" s="5">
         <f t="shared" si="0"/>
         <v>13.779527559055119</v>
       </c>
-      <c r="L37" s="7">
+      <c r="M37" s="5">
         <f t="shared" si="0"/>
         <v>10.60944881889764</v>
       </c>
-      <c r="M37" s="8" t="s">
+      <c r="N37" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
         <v>15</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C38" s="4">
         <v>9</v>
       </c>
@@ -1170,37 +1210,40 @@
       <c r="F38" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I38" s="3">
+      <c r="J38" s="3">
         <v>1201.6600000000001</v>
       </c>
-      <c r="J38" s="3">
+      <c r="K38" s="3">
         <v>201.66</v>
       </c>
-      <c r="K38" s="7">
+      <c r="L38" s="5">
         <f t="shared" si="0"/>
         <v>47.309448818897643</v>
       </c>
-      <c r="L38" s="7">
+      <c r="M38" s="5">
         <f t="shared" si="0"/>
         <v>7.9393700787401578</v>
       </c>
-      <c r="M38" s="8" t="s">
+      <c r="N38" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O38" s="1" t="s">
+      <c r="P38" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C39" s="4">
         <v>10</v>
       </c>
@@ -1213,37 +1256,40 @@
       <c r="F39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I39" s="3">
+      <c r="J39" s="3">
         <v>981.66</v>
       </c>
-      <c r="J39" s="3">
+      <c r="K39" s="3">
         <v>211.01</v>
       </c>
-      <c r="K39" s="7">
+      <c r="L39" s="5">
         <f t="shared" si="0"/>
         <v>38.648031496062991</v>
       </c>
-      <c r="L39" s="7">
+      <c r="M39" s="5">
         <f t="shared" si="0"/>
         <v>8.30748031496063</v>
       </c>
-      <c r="M39" s="8" t="s">
+      <c r="N39" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O39" s="1" t="s">
+      <c r="P39" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C40" s="4">
         <v>11</v>
       </c>
@@ -1256,34 +1302,37 @@
       <c r="F40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="3">
+      <c r="J40" s="3">
         <v>331.78</v>
       </c>
-      <c r="J40" s="3">
+      <c r="K40" s="3">
         <v>216.31</v>
       </c>
-      <c r="K40" s="7">
+      <c r="L40" s="5">
         <f t="shared" si="0"/>
         <v>13.062204724409449</v>
       </c>
-      <c r="L40" s="7">
+      <c r="M40" s="5">
         <f t="shared" si="0"/>
         <v>8.5161417322834652</v>
       </c>
-      <c r="M40" s="8" t="s">
+      <c r="N40" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O40" s="1" t="s">
+      <c r="P40" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C41" s="4">
         <v>12</v>
       </c>
@@ -1296,34 +1345,37 @@
       <c r="F41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I41" s="3">
+      <c r="J41" s="3">
         <v>30</v>
       </c>
-      <c r="J41" s="3">
+      <c r="K41" s="3">
         <v>91.25</v>
       </c>
-      <c r="K41" s="7">
+      <c r="L41" s="5">
         <f t="shared" si="0"/>
         <v>1.1811023622047245</v>
       </c>
-      <c r="L41" s="7">
+      <c r="M41" s="5">
         <f t="shared" si="0"/>
         <v>3.5925196850393704</v>
       </c>
-      <c r="M41" s="8" t="s">
+      <c r="N41" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="O41" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O41" s="1" t="s">
+      <c r="P41" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C42" s="4">
         <v>13</v>
       </c>
@@ -1336,72 +1388,75 @@
       <c r="F42" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="3">
+      <c r="J42" s="3">
         <v>66</v>
       </c>
-      <c r="J42" s="3">
+      <c r="K42" s="3">
         <v>118.83</v>
       </c>
-      <c r="K42" s="7">
+      <c r="L42" s="5">
         <f t="shared" si="0"/>
         <v>2.598425196850394</v>
       </c>
-      <c r="L42" s="7">
+      <c r="M42" s="5">
         <f t="shared" si="0"/>
         <v>4.6783464566929132</v>
       </c>
-      <c r="M42" s="8" t="s">
+      <c r="N42" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O42" s="1" t="s">
+      <c r="P42" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="10">
-        <f>SUMPRODUCT(K30:K36,L30:L36,E30:E36)</f>
+    <row r="45" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C45" s="8">
+        <f>SUMPRODUCT(L30:L36,M30:M36,E30:E36)</f>
         <v>2174.1645805691614</v>
       </c>
       <c r="D45" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C47" s="10">
-        <f>SUMPRODUCT(L37:L39,K37:K39,E37:E39)</f>
+    <row r="47" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C47" s="8">
+        <f>SUMPRODUCT(M37:M39,L37:L39,E37:E39)</f>
         <v>842.86817564635135</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="10">
-        <f>SUMPRODUCT(E40:E42,K40:K42,L40:L42)</f>
+      <c r="C49" s="8">
+        <f>SUMPRODUCT(E40:E42,L40:L42,M40:M42)</f>
         <v>243.12177382354767</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1410,13 +1465,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F5:L5"/>
-    <mergeCell ref="F6:L6"/>
-    <mergeCell ref="F7:L7"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="F16:L16"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="F5:M5"/>
+    <mergeCell ref="F6:M6"/>
+    <mergeCell ref="F7:M7"/>
+    <mergeCell ref="F8:M8"/>
+    <mergeCell ref="F16:M16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Final update of first version
Will revision for cost reduction and DFM
</commit_message>
<xml_diff>
--- a/export/SM_BOM.xlsx
+++ b/export/SM_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" tabRatio="284"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="90">
   <si>
     <t>Item #</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Deburr, vertically brushed finish, will eveutually be annodized.</t>
-  </si>
-  <si>
     <t>Part number</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Raw</t>
   </si>
   <si>
-    <t>Plated</t>
-  </si>
-  <si>
     <t>Material Details</t>
   </si>
   <si>
@@ -216,13 +210,82 @@
     <t>square inch</t>
   </si>
   <si>
-    <t>TBD, assume black</t>
-  </si>
-  <si>
     <t>Revision</t>
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>Preplated</t>
+  </si>
+  <si>
+    <t>TBD, assume none</t>
+  </si>
+  <si>
+    <t>Weldment remarks</t>
+  </si>
+  <si>
+    <t>No welds</t>
+  </si>
+  <si>
+    <t>Spot welds</t>
+  </si>
+  <si>
+    <t>Spot weld seam for rigidity</t>
+  </si>
+  <si>
+    <t>See drawer for welding details</t>
+  </si>
+  <si>
+    <t>Full seam weld for watertight</t>
+  </si>
+  <si>
+    <t>Full seam weld for visual appeal</t>
+  </si>
+  <si>
+    <t>1k cost</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>projected</t>
+  </si>
+  <si>
+    <t>Remove circular fold</t>
+  </si>
+  <si>
+    <t>Change tools, allow bigger tools</t>
+  </si>
+  <si>
+    <t>Rivots</t>
+  </si>
+  <si>
+    <t>no change</t>
+  </si>
+  <si>
+    <t>Steel?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>steel</t>
+  </si>
+  <si>
+    <t>convert to rivot</t>
+  </si>
+  <si>
+    <t>no welds</t>
+  </si>
+  <si>
+    <t>raw $</t>
+  </si>
+  <si>
+    <t>aluminum</t>
+  </si>
+  <si>
+    <t>per sqin</t>
   </si>
 </sst>
 </file>
@@ -586,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:P49"/>
+  <dimension ref="C1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="Q19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W45" sqref="W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,28 +665,33 @@
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="13" width="18.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="16" style="1" customWidth="1"/>
-    <col min="15" max="15" width="61" customWidth="1"/>
+    <col min="15" max="15" width="21.28515625" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
+    <col min="17" max="17" width="43.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" customWidth="1"/>
+    <col min="19" max="19" width="35.7109375" customWidth="1"/>
+    <col min="21" max="21" width="37.42578125" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -635,10 +703,10 @@
     </row>
     <row r="6" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
@@ -650,10 +718,10 @@
     </row>
     <row r="7" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -665,10 +733,10 @@
     </row>
     <row r="8" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -710,15 +778,15 @@
     </row>
     <row r="15" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>60</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
@@ -728,27 +796,27 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -758,34 +826,56 @@
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W24" s="1">
+        <f>75/48/96</f>
+        <v>1.6276041666666668E-2</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="W25" s="1">
+        <f>50/48/96</f>
+        <v>1.0850694444444446E-2</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="3:24" x14ac:dyDescent="0.25">
       <c r="J28" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K28" s="9"/>
       <c r="L28" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M28" s="9"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
@@ -796,40 +886,61 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="L29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="N29" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>68</v>
+      </c>
+      <c r="R29" t="s">
+        <v>75</v>
+      </c>
+      <c r="S29" t="s">
+        <v>76</v>
+      </c>
+      <c r="T29" t="s">
+        <v>77</v>
+      </c>
+      <c r="U29" t="s">
+        <v>76</v>
+      </c>
+      <c r="V29" t="s">
+        <v>77</v>
+      </c>
+      <c r="W29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C30" s="4">
         <v>1</v>
       </c>
@@ -840,16 +951,16 @@
         <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H30" t="s">
         <v>10</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J30" s="3">
         <v>194.48</v>
@@ -866,16 +977,35 @@
         <v>11.593700787401577</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O30" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="P30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>69</v>
+      </c>
+      <c r="R30">
+        <v>22</v>
+      </c>
+      <c r="S30" t="s">
+        <v>79</v>
+      </c>
+      <c r="T30">
+        <v>12</v>
+      </c>
+      <c r="V30">
+        <v>12</v>
+      </c>
+      <c r="W30">
+        <f>L30*M30*W$24</f>
+        <v>1.4448145615041235</v>
+      </c>
+    </row>
+    <row r="31" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C31" s="4">
         <v>2</v>
       </c>
@@ -886,16 +1016,16 @@
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J31" s="3">
         <v>464.48</v>
@@ -912,16 +1042,35 @@
         <v>8.1385826771653544</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>70</v>
+      </c>
+      <c r="R31">
+        <v>26</v>
+      </c>
+      <c r="S31" t="s">
+        <v>80</v>
+      </c>
+      <c r="T31">
+        <v>12</v>
+      </c>
+      <c r="V31">
+        <v>12</v>
+      </c>
+      <c r="W31" s="1">
+        <f t="shared" ref="W31:W36" si="1">L31*M31*W$24</f>
+        <v>2.42231642796619</v>
+      </c>
+    </row>
+    <row r="32" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C32" s="4">
         <v>3</v>
       </c>
@@ -932,16 +1081,16 @@
         <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J32" s="3">
         <v>407.66</v>
@@ -958,16 +1107,32 @@
         <v>17.018110236220473</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>71</v>
+      </c>
+      <c r="R32">
+        <v>32</v>
+      </c>
+      <c r="T32">
+        <v>8</v>
+      </c>
+      <c r="V32">
+        <v>8</v>
+      </c>
+      <c r="W32" s="1">
+        <f t="shared" si="1"/>
+        <v>4.4455398640615007</v>
+      </c>
+    </row>
+    <row r="33" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C33" s="4">
         <v>4</v>
       </c>
@@ -978,16 +1143,16 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J33" s="3">
         <v>407.66</v>
@@ -1004,16 +1169,32 @@
         <v>17.018110236220473</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R33">
+        <v>32</v>
+      </c>
+      <c r="T33">
+        <v>8</v>
+      </c>
+      <c r="V33">
+        <v>8</v>
+      </c>
+      <c r="W33" s="1">
+        <f t="shared" si="1"/>
+        <v>4.4455398640615007</v>
+      </c>
+    </row>
+    <row r="34" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C34" s="4">
         <v>5</v>
       </c>
@@ -1024,16 +1205,16 @@
         <v>2</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J34" s="3">
         <v>704.42</v>
@@ -1050,16 +1231,38 @@
         <v>17.159842519685039</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R34">
+        <v>30</v>
+      </c>
+      <c r="S34" t="s">
+        <v>81</v>
+      </c>
+      <c r="T34">
+        <v>30</v>
+      </c>
+      <c r="U34" t="s">
+        <v>86</v>
+      </c>
+      <c r="V34">
+        <v>15</v>
+      </c>
+      <c r="W34" s="1">
+        <f t="shared" si="1"/>
+        <v>7.7456889428752813</v>
+      </c>
+    </row>
+    <row r="35" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C35" s="4">
         <v>6</v>
       </c>
@@ -1070,16 +1273,16 @@
         <v>2</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J35" s="3">
         <v>323.14</v>
@@ -1096,36 +1299,58 @@
         <v>12.722047244094489</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>73</v>
+      </c>
+      <c r="R35">
+        <v>38</v>
+      </c>
+      <c r="S35" t="s">
+        <v>82</v>
+      </c>
+      <c r="T35">
+        <v>38</v>
+      </c>
+      <c r="U35" t="s">
+        <v>84</v>
+      </c>
+      <c r="V35">
+        <v>30</v>
+      </c>
+      <c r="W35" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6342852552241562</v>
+      </c>
+    </row>
+    <row r="36" spans="3:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="4">
         <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E36" s="4">
         <v>1</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J36" s="3">
         <v>251</v>
@@ -1142,16 +1367,35 @@
         <v>11.618110236220474</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R36" s="1">
+        <v>6</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="T36" s="1">
+        <v>6</v>
+      </c>
+      <c r="V36" s="1">
+        <v>6</v>
+      </c>
+      <c r="W36" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8686341897423382</v>
+      </c>
+    </row>
+    <row r="37" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C37" s="4">
         <v>8</v>
       </c>
@@ -1162,16 +1406,16 @@
         <v>1</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H37" t="s">
         <v>14</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="J37" s="3">
         <v>350</v>
@@ -1188,16 +1432,38 @@
         <v>10.60944881889764</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O37" t="s">
         <v>15</v>
       </c>
       <c r="P37" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R37">
+        <v>26</v>
+      </c>
+      <c r="S37" t="s">
+        <v>83</v>
+      </c>
+      <c r="T37">
+        <v>26</v>
+      </c>
+      <c r="U37" t="s">
+        <v>85</v>
+      </c>
+      <c r="V37">
+        <v>13</v>
+      </c>
+      <c r="W37" s="1">
+        <f>L37*M37*W$25</f>
+        <v>1.5862976604425436</v>
+      </c>
+    </row>
+    <row r="38" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C38" s="4">
         <v>9</v>
       </c>
@@ -1208,16 +1474,16 @@
         <v>1</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="J38" s="3">
         <v>1201.6600000000001</v>
@@ -1234,16 +1500,35 @@
         <v>7.9393700787401578</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>71</v>
+      </c>
+      <c r="R38">
+        <v>50</v>
+      </c>
+      <c r="S38" t="s">
+        <v>80</v>
+      </c>
+      <c r="T38">
+        <v>15</v>
+      </c>
+      <c r="V38">
+        <v>15</v>
+      </c>
+      <c r="W38" s="1">
+        <f t="shared" ref="W38:W42" si="2">L38*M38*W$25</f>
+        <v>4.075599201328612</v>
+      </c>
+    </row>
+    <row r="39" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C39" s="4">
         <v>10</v>
       </c>
@@ -1254,16 +1539,16 @@
         <v>1</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="J39" s="3">
         <v>981.66</v>
@@ -1280,16 +1565,35 @@
         <v>8.30748031496063</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O39" s="1" t="s">
         <v>15</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R39">
+        <v>53</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T39">
+        <v>15</v>
+      </c>
+      <c r="V39">
+        <v>15</v>
+      </c>
+      <c r="W39" s="1">
+        <f t="shared" si="2"/>
+        <v>3.4838081691137344</v>
+      </c>
+    </row>
+    <row r="40" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C40" s="4">
         <v>11</v>
       </c>
@@ -1300,10 +1604,10 @@
         <v>2</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H40" t="s">
         <v>19</v>
@@ -1323,16 +1627,35 @@
         <v>8.5161417322834652</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="3:16" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R40">
+        <v>6</v>
+      </c>
+      <c r="S40" t="s">
+        <v>81</v>
+      </c>
+      <c r="T40">
+        <v>6</v>
+      </c>
+      <c r="V40">
+        <v>6</v>
+      </c>
+      <c r="W40" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2070267661585674</v>
+      </c>
+    </row>
+    <row r="41" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C41" s="4">
         <v>12</v>
       </c>
@@ -1343,10 +1666,10 @@
         <v>2</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>19</v>
@@ -1366,16 +1689,35 @@
         <v>3.5925196850393704</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O41" s="1" t="s">
         <v>15</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="3:16" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R41">
+        <v>27</v>
+      </c>
+      <c r="S41" t="s">
+        <v>78</v>
+      </c>
+      <c r="T41">
+        <v>3</v>
+      </c>
+      <c r="V41">
+        <v>3</v>
+      </c>
+      <c r="W41" s="1">
+        <f t="shared" si="2"/>
+        <v>4.604094494647324E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C42" s="4">
         <v>13</v>
       </c>
@@ -1386,10 +1728,10 @@
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>19</v>
@@ -1409,49 +1751,84 @@
         <v>4.6783464566929132</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O42" s="1" t="s">
         <v>15</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="3:16" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R42">
+        <v>1</v>
+      </c>
+      <c r="S42" t="s">
+        <v>81</v>
+      </c>
+      <c r="T42">
+        <v>1</v>
+      </c>
+      <c r="V42">
+        <v>1</v>
+      </c>
+      <c r="W42" s="1">
+        <f t="shared" si="2"/>
+        <v>0.13190465834056672</v>
+      </c>
+    </row>
+    <row r="43" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="3:16" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="R44">
+        <f>SUMPRODUCT(R30:R42,E30:E42)</f>
+        <v>450</v>
+      </c>
+      <c r="T44">
+        <f>SUMPRODUCT(T30:T42,E30:E42)</f>
+        <v>257</v>
+      </c>
+      <c r="V44">
+        <f>SUMPRODUCT(V30:V42,E30:E42)</f>
+        <v>198</v>
+      </c>
+      <c r="W44">
+        <f>SUMPRODUCT(W30:W42,E30:E42)</f>
+        <v>47.170538414970068</v>
+      </c>
+    </row>
+    <row r="45" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C45" s="8">
         <f>SUMPRODUCT(L30:L36,M30:M36,E30:E36)</f>
         <v>2174.1645805691614</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="3:16" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="3:16" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C47" s="8">
         <f>SUMPRODUCT(M37:M39,L37:L39,E37:E39)</f>
         <v>842.86817564635135</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="3:16" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
@@ -1460,7 +1837,7 @@
         <v>243.12177382354767</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cost reduction round 1
</commit_message>
<xml_diff>
--- a/export/SM_BOM.xlsx
+++ b/export/SM_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="77">
   <si>
     <t>Item #</t>
   </si>
@@ -228,64 +228,25 @@
     <t>No welds</t>
   </si>
   <si>
-    <t>Spot welds</t>
-  </si>
-  <si>
-    <t>Spot weld seam for rigidity</t>
-  </si>
-  <si>
-    <t>See drawer for welding details</t>
-  </si>
-  <si>
     <t>Full seam weld for watertight</t>
   </si>
   <si>
-    <t>Full seam weld for visual appeal</t>
-  </si>
-  <si>
-    <t>1k cost</t>
-  </si>
-  <si>
     <t>edit</t>
   </si>
   <si>
-    <t>projected</t>
-  </si>
-  <si>
-    <t>Remove circular fold</t>
-  </si>
-  <si>
-    <t>Change tools, allow bigger tools</t>
-  </si>
-  <si>
-    <t>Rivots</t>
-  </si>
-  <si>
     <t>no change</t>
   </si>
   <si>
-    <t>Steel?</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>steel</t>
-  </si>
-  <si>
-    <t>convert to rivot</t>
-  </si>
-  <si>
-    <t>no welds</t>
-  </si>
-  <si>
-    <t>raw $</t>
-  </si>
-  <si>
-    <t>aluminum</t>
-  </si>
-  <si>
-    <t>per sqin</t>
+    <t>Replaced welds with rivets</t>
+  </si>
+  <si>
+    <t>Remove welds</t>
+  </si>
+  <si>
+    <t>Replace circular with normal bends</t>
+  </si>
+  <si>
+    <t>1.1</t>
   </si>
 </sst>
 </file>
@@ -324,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -346,8 +307,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:X49"/>
+  <dimension ref="C1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W45" sqref="W45"/>
+    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,10 +633,8 @@
     <col min="15" max="15" width="21.28515625" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
     <col min="17" max="17" width="43.7109375" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" customWidth="1"/>
-    <col min="19" max="19" width="35.7109375" customWidth="1"/>
-    <col min="21" max="21" width="37.42578125" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" customWidth="1"/>
+    <col min="18" max="18" width="41.85546875" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -690,61 +653,61 @@
       <c r="D5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
     </row>
     <row r="6" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
     </row>
     <row r="7" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
@@ -785,33 +748,33 @@
       <c r="D16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-    </row>
-    <row r="17" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
         <v>57</v>
       </c>
@@ -826,56 +789,34 @@
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="V24" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="W24" s="1">
-        <f>75/48/96</f>
-        <v>1.6276041666666668E-2</v>
-      </c>
-      <c r="X24" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="3:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="V25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="W25" s="1">
-        <f>50/48/96</f>
-        <v>1.0850694444444446E-2</v>
-      </c>
-      <c r="X25" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="J28" s="9" t="s">
+    <row r="24" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="J28" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9" t="s">
+      <c r="K28" s="10"/>
+      <c r="L28" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="M28" s="9"/>
-    </row>
-    <row r="29" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="M28" s="10"/>
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,25 +863,10 @@
         <v>68</v>
       </c>
       <c r="R29" t="s">
-        <v>75</v>
-      </c>
-      <c r="S29" t="s">
-        <v>76</v>
-      </c>
-      <c r="T29" t="s">
-        <v>77</v>
-      </c>
-      <c r="U29" t="s">
-        <v>76</v>
-      </c>
-      <c r="V29" t="s">
-        <v>77</v>
-      </c>
-      <c r="W29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="3:24" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C30" s="4">
         <v>1</v>
       </c>
@@ -954,7 +880,7 @@
         <v>22</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H30" t="s">
         <v>10</v>
@@ -988,24 +914,12 @@
       <c r="Q30" t="s">
         <v>69</v>
       </c>
-      <c r="R30">
-        <v>22</v>
-      </c>
-      <c r="S30" t="s">
-        <v>79</v>
-      </c>
-      <c r="T30">
-        <v>12</v>
-      </c>
-      <c r="V30">
-        <v>12</v>
-      </c>
-      <c r="W30">
-        <f>L30*M30*W$24</f>
-        <v>1.4448145615041235</v>
-      </c>
-    </row>
-    <row r="31" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="R30" t="s">
+        <v>73</v>
+      </c>
+      <c r="S30" s="12"/>
+    </row>
+    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C31" s="4">
         <v>2</v>
       </c>
@@ -1019,7 +933,7 @@
         <v>23</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>10</v>
@@ -1050,27 +964,15 @@
       <c r="P31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q31" t="s">
-        <v>70</v>
-      </c>
-      <c r="R31">
-        <v>26</v>
-      </c>
-      <c r="S31" t="s">
-        <v>80</v>
-      </c>
-      <c r="T31">
-        <v>12</v>
-      </c>
-      <c r="V31">
-        <v>12</v>
-      </c>
-      <c r="W31" s="1">
-        <f t="shared" ref="W31:W36" si="1">L31*M31*W$24</f>
-        <v>2.42231642796619</v>
-      </c>
-    </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="Q31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S31" s="12"/>
+    </row>
+    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C32" s="4">
         <v>3</v>
       </c>
@@ -1084,7 +986,7 @@
         <v>24</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>10</v>
@@ -1093,18 +995,18 @@
         <v>50</v>
       </c>
       <c r="J32" s="3">
-        <v>407.66</v>
+        <v>360.65</v>
       </c>
       <c r="K32" s="3">
-        <v>432.26</v>
+        <v>425.43</v>
       </c>
       <c r="L32" s="5">
         <f t="shared" si="0"/>
-        <v>16.049606299212602</v>
+        <v>14.198818897637794</v>
       </c>
       <c r="M32" s="5">
         <f t="shared" si="0"/>
-        <v>17.018110236220473</v>
+        <v>16.749212598425199</v>
       </c>
       <c r="N32" s="6" t="s">
         <v>55</v>
@@ -1115,24 +1017,15 @@
       <c r="P32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q32" t="s">
-        <v>71</v>
-      </c>
-      <c r="R32">
-        <v>32</v>
-      </c>
-      <c r="T32">
-        <v>8</v>
-      </c>
-      <c r="V32">
-        <v>8</v>
-      </c>
-      <c r="W32" s="1">
-        <f t="shared" si="1"/>
-        <v>4.4455398640615007</v>
-      </c>
-    </row>
-    <row r="33" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Q32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S32" s="12"/>
+    </row>
+    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C33" s="4">
         <v>4</v>
       </c>
@@ -1146,7 +1039,7 @@
         <v>25</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>10</v>
@@ -1154,19 +1047,19 @@
       <c r="I33" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J33" s="3">
-        <v>407.66</v>
-      </c>
-      <c r="K33" s="3">
-        <v>432.26</v>
+      <c r="J33" s="9">
+        <v>360.65</v>
+      </c>
+      <c r="K33" s="9">
+        <v>425.43</v>
       </c>
       <c r="L33" s="5">
         <f t="shared" si="0"/>
-        <v>16.049606299212602</v>
+        <v>14.198818897637794</v>
       </c>
       <c r="M33" s="5">
         <f t="shared" si="0"/>
-        <v>17.018110236220473</v>
+        <v>16.749212598425199</v>
       </c>
       <c r="N33" s="6" t="s">
         <v>55</v>
@@ -1178,23 +1071,14 @@
         <v>67</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R33">
-        <v>32</v>
-      </c>
-      <c r="T33">
-        <v>8</v>
-      </c>
-      <c r="V33">
-        <v>8</v>
-      </c>
-      <c r="W33" s="1">
-        <f t="shared" si="1"/>
-        <v>4.4455398640615007</v>
-      </c>
-    </row>
-    <row r="34" spans="3:23" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S33" s="12"/>
+    </row>
+    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C34" s="4">
         <v>5</v>
       </c>
@@ -1208,7 +1092,7 @@
         <v>26</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>10</v>
@@ -1220,7 +1104,7 @@
         <v>704.42</v>
       </c>
       <c r="K34" s="3">
-        <v>435.86</v>
+        <v>437.86</v>
       </c>
       <c r="L34" s="5">
         <f t="shared" si="0"/>
@@ -1228,7 +1112,7 @@
       </c>
       <c r="M34" s="5">
         <f t="shared" si="0"/>
-        <v>17.159842519685039</v>
+        <v>17.238582677165354</v>
       </c>
       <c r="N34" s="6" t="s">
         <v>55</v>
@@ -1240,29 +1124,14 @@
         <v>67</v>
       </c>
       <c r="Q34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R34" t="s">
         <v>74</v>
       </c>
-      <c r="R34">
-        <v>30</v>
-      </c>
-      <c r="S34" t="s">
-        <v>81</v>
-      </c>
-      <c r="T34">
-        <v>30</v>
-      </c>
-      <c r="U34" t="s">
-        <v>86</v>
-      </c>
-      <c r="V34">
-        <v>15</v>
-      </c>
-      <c r="W34" s="1">
-        <f t="shared" si="1"/>
-        <v>7.7456889428752813</v>
-      </c>
-    </row>
-    <row r="35" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="S34" s="12"/>
+    </row>
+    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C35" s="4">
         <v>6</v>
       </c>
@@ -1276,7 +1145,7 @@
         <v>27</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>10</v>
@@ -1308,29 +1177,11 @@
         <v>67</v>
       </c>
       <c r="Q35" t="s">
-        <v>73</v>
-      </c>
-      <c r="R35">
-        <v>38</v>
-      </c>
-      <c r="S35" t="s">
-        <v>82</v>
-      </c>
-      <c r="T35">
-        <v>38</v>
-      </c>
-      <c r="U35" t="s">
-        <v>84</v>
-      </c>
-      <c r="V35">
-        <v>30</v>
-      </c>
-      <c r="W35" s="1">
-        <f t="shared" si="1"/>
-        <v>2.6342852552241562</v>
-      </c>
-    </row>
-    <row r="36" spans="3:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="S35" s="12"/>
+    </row>
+    <row r="36" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="4">
         <v>7</v>
       </c>
@@ -1378,24 +1229,12 @@
       <c r="Q36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R36" s="1">
-        <v>6</v>
-      </c>
-      <c r="S36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="T36" s="1">
-        <v>6</v>
-      </c>
-      <c r="V36" s="1">
-        <v>6</v>
-      </c>
-      <c r="W36" s="1">
-        <f t="shared" si="1"/>
-        <v>1.8686341897423382</v>
-      </c>
-    </row>
-    <row r="37" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S36" s="12"/>
+    </row>
+    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C37" s="4">
         <v>8</v>
       </c>
@@ -1409,7 +1248,7 @@
         <v>29</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H37" t="s">
         <v>14</v>
@@ -1441,29 +1280,14 @@
         <v>53</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="R37">
-        <v>26</v>
-      </c>
-      <c r="S37" t="s">
-        <v>83</v>
-      </c>
-      <c r="T37">
-        <v>26</v>
-      </c>
-      <c r="U37" t="s">
-        <v>85</v>
-      </c>
-      <c r="V37">
-        <v>13</v>
-      </c>
-      <c r="W37" s="1">
-        <f>L37*M37*W$25</f>
-        <v>1.5862976604425436</v>
-      </c>
-    </row>
-    <row r="38" spans="3:23" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S37" s="12"/>
+    </row>
+    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C38" s="4">
         <v>9</v>
       </c>
@@ -1477,7 +1301,7 @@
         <v>30</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>14</v>
@@ -1489,7 +1313,7 @@
         <v>1201.6600000000001</v>
       </c>
       <c r="K38" s="3">
-        <v>201.66</v>
+        <v>208.01</v>
       </c>
       <c r="L38" s="5">
         <f t="shared" si="0"/>
@@ -1497,7 +1321,7 @@
       </c>
       <c r="M38" s="5">
         <f t="shared" si="0"/>
-        <v>7.9393700787401578</v>
+        <v>8.1893700787401578</v>
       </c>
       <c r="N38" s="6" t="s">
         <v>55</v>
@@ -1508,27 +1332,15 @@
       <c r="P38" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q38" t="s">
-        <v>71</v>
-      </c>
-      <c r="R38">
-        <v>50</v>
-      </c>
-      <c r="S38" t="s">
-        <v>80</v>
-      </c>
-      <c r="T38">
-        <v>15</v>
-      </c>
-      <c r="V38">
-        <v>15</v>
-      </c>
-      <c r="W38" s="1">
-        <f t="shared" ref="W38:W42" si="2">L38*M38*W$25</f>
-        <v>4.075599201328612</v>
-      </c>
-    </row>
-    <row r="39" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Q38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S38" s="12"/>
+    </row>
+    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C39" s="4">
         <v>10</v>
       </c>
@@ -1542,7 +1354,7 @@
         <v>31</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -1574,26 +1386,14 @@
         <v>53</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="R39">
-        <v>53</v>
-      </c>
-      <c r="S39" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="T39">
-        <v>15</v>
-      </c>
-      <c r="V39">
-        <v>15</v>
-      </c>
-      <c r="W39" s="1">
-        <f t="shared" si="2"/>
-        <v>3.4838081691137344</v>
-      </c>
-    </row>
-    <row r="40" spans="3:23" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S39" s="12"/>
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C40" s="4">
         <v>11</v>
       </c>
@@ -1607,7 +1407,7 @@
         <v>32</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H40" t="s">
         <v>19</v>
@@ -1638,24 +1438,12 @@
       <c r="Q40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R40">
-        <v>6</v>
-      </c>
-      <c r="S40" t="s">
-        <v>81</v>
-      </c>
-      <c r="T40">
-        <v>6</v>
-      </c>
-      <c r="V40">
-        <v>6</v>
-      </c>
-      <c r="W40" s="1">
-        <f t="shared" si="2"/>
-        <v>1.2070267661585674</v>
-      </c>
-    </row>
-    <row r="41" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R40" t="s">
+        <v>72</v>
+      </c>
+      <c r="S40" s="12"/>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C41" s="4">
         <v>12</v>
       </c>
@@ -1669,7 +1457,7 @@
         <v>33</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>19</v>
@@ -1678,7 +1466,7 @@
         <v>30</v>
       </c>
       <c r="K41" s="3">
-        <v>91.25</v>
+        <v>92.19</v>
       </c>
       <c r="L41" s="5">
         <f t="shared" si="0"/>
@@ -1686,7 +1474,7 @@
       </c>
       <c r="M41" s="5">
         <f t="shared" si="0"/>
-        <v>3.5925196850393704</v>
+        <v>3.6295275590551181</v>
       </c>
       <c r="N41" s="6" t="s">
         <v>55</v>
@@ -1700,24 +1488,12 @@
       <c r="Q41" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R41">
-        <v>27</v>
-      </c>
-      <c r="S41" t="s">
-        <v>78</v>
-      </c>
-      <c r="T41">
-        <v>3</v>
-      </c>
-      <c r="V41">
-        <v>3</v>
-      </c>
-      <c r="W41" s="1">
-        <f t="shared" si="2"/>
-        <v>4.604094494647324E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R41" t="s">
+        <v>75</v>
+      </c>
+      <c r="S41" s="12"/>
+    </row>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C42" s="4">
         <v>13</v>
       </c>
@@ -1762,71 +1538,45 @@
       <c r="Q42" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R42">
-        <v>1</v>
-      </c>
-      <c r="S42" t="s">
-        <v>81</v>
-      </c>
-      <c r="T42">
-        <v>1</v>
-      </c>
-      <c r="V42">
-        <v>1</v>
-      </c>
-      <c r="W42" s="1">
-        <f t="shared" si="2"/>
-        <v>0.13190465834056672</v>
-      </c>
-    </row>
-    <row r="43" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R42" t="s">
+        <v>72</v>
+      </c>
+      <c r="S42" s="12"/>
+    </row>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="S43" s="12"/>
+    </row>
+    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R44">
-        <f>SUMPRODUCT(R30:R42,E30:E42)</f>
-        <v>450</v>
-      </c>
-      <c r="T44">
-        <f>SUMPRODUCT(T30:T42,E30:E42)</f>
-        <v>257</v>
-      </c>
-      <c r="V44">
-        <f>SUMPRODUCT(V30:V42,E30:E42)</f>
-        <v>198</v>
-      </c>
-      <c r="W44">
-        <f>SUMPRODUCT(W30:W42,E30:E42)</f>
-        <v>47.170538414970068</v>
-      </c>
-    </row>
-    <row r="45" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="S44" s="12"/>
+    </row>
+    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C45" s="8">
         <f>SUMPRODUCT(L30:L36,M30:M36,E30:E36)</f>
-        <v>2174.1645805691614</v>
+        <v>2107.9021275342552</v>
       </c>
       <c r="D45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C47" s="8">
         <f>SUMPRODUCT(M37:M39,L37:L39,E37:E39)</f>
-        <v>842.86817564635135</v>
+        <v>854.69553785107564</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>62</v>
       </c>
@@ -1834,7 +1584,7 @@
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="8">
         <f>SUMPRODUCT(E40:E42,L40:L42,M40:M42)</f>
-        <v>243.12177382354767</v>
+        <v>243.20919399838803</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Reduced number of unique tools
</commit_message>
<xml_diff>
--- a/export/SM_BOM.xlsx
+++ b/export/SM_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="92">
   <si>
     <t>Item #</t>
   </si>
@@ -222,15 +222,6 @@
     <t>TBD, assume none</t>
   </si>
   <si>
-    <t>Weldment remarks</t>
-  </si>
-  <si>
-    <t>No welds</t>
-  </si>
-  <si>
-    <t>Full seam weld for watertight</t>
-  </si>
-  <si>
     <t>edit</t>
   </si>
   <si>
@@ -247,6 +238,60 @@
   </si>
   <si>
     <t>1.1</t>
+  </si>
+  <si>
+    <t>Full seam weld for watertight seam</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>usage</t>
+  </si>
+  <si>
+    <t>M3 screw</t>
+  </si>
+  <si>
+    <t>1/8" rivet</t>
+  </si>
+  <si>
+    <t>M3 press nut</t>
+  </si>
+  <si>
+    <t>M5 press nut</t>
+  </si>
+  <si>
+    <t>M5 screw</t>
+  </si>
+  <si>
+    <t>8mm linear bearing</t>
+  </si>
+  <si>
+    <t>Welding</t>
+  </si>
+  <si>
+    <t>Round</t>
+  </si>
+  <si>
+    <t>Diameter (mm)</t>
+  </si>
+  <si>
+    <t>Alternative (in)</t>
+  </si>
+  <si>
+    <t>Obround</t>
+  </si>
+  <si>
+    <t>0.120 x 0.238</t>
+  </si>
+  <si>
+    <t>0.156 x 0.276</t>
+  </si>
+  <si>
+    <t>M3 screw slot</t>
+  </si>
+  <si>
+    <t>M4 screw slot</t>
   </si>
 </sst>
 </file>
@@ -306,13 +351,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,25 +659,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:S49"/>
+  <dimension ref="C1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="13" width="18.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="16" style="1" customWidth="1"/>
     <col min="15" max="15" width="21.28515625" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
-    <col min="17" max="17" width="43.7109375" customWidth="1"/>
+    <col min="17" max="17" width="35" customWidth="1"/>
     <col min="18" max="18" width="41.85546875" customWidth="1"/>
     <col min="20" max="20" width="14.28515625" customWidth="1"/>
   </cols>
@@ -653,61 +698,61 @@
       <c r="D5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
     </row>
     <row r="7" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
     </row>
     <row r="8" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
@@ -748,16 +793,16 @@
       <c r="D16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
@@ -807,14 +852,14 @@
     <row r="24" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="J28" s="10" t="s">
+      <c r="J28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10" t="s">
+      <c r="K28" s="11"/>
+      <c r="L28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="M28" s="10"/>
+      <c r="M28" s="11"/>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
@@ -860,10 +905,10 @@
         <v>52</v>
       </c>
       <c r="Q29" t="s">
+        <v>83</v>
+      </c>
+      <c r="R29" t="s">
         <v>68</v>
-      </c>
-      <c r="R29" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.25">
@@ -880,7 +925,7 @@
         <v>22</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H30" t="s">
         <v>10</v>
@@ -911,13 +956,13 @@
       <c r="P30" t="s">
         <v>67</v>
       </c>
-      <c r="Q30" t="s">
-        <v>69</v>
+      <c r="Q30" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="R30" t="s">
-        <v>73</v>
-      </c>
-      <c r="S30" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="S30" s="10"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C31" s="4">
@@ -933,7 +978,7 @@
         <v>23</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>10</v>
@@ -965,12 +1010,12 @@
         <v>67</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S31" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="S31" s="10"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C32" s="4">
@@ -986,7 +1031,7 @@
         <v>24</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>10</v>
@@ -1018,12 +1063,12 @@
         <v>67</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S32" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="S32" s="10"/>
     </row>
     <row r="33" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C33" s="4">
@@ -1039,7 +1084,7 @@
         <v>25</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>10</v>
@@ -1071,12 +1116,12 @@
         <v>67</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S33" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="S33" s="10"/>
     </row>
     <row r="34" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C34" s="4">
@@ -1092,7 +1137,7 @@
         <v>26</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>10</v>
@@ -1124,12 +1169,12 @@
         <v>67</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="R34" t="s">
-        <v>74</v>
-      </c>
-      <c r="S34" s="12"/>
+        <v>71</v>
+      </c>
+      <c r="S34" s="10"/>
     </row>
     <row r="35" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C35" s="4">
@@ -1145,7 +1190,7 @@
         <v>27</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>10</v>
@@ -1177,9 +1222,9 @@
         <v>67</v>
       </c>
       <c r="Q35" t="s">
-        <v>70</v>
-      </c>
-      <c r="S35" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="S35" s="10"/>
     </row>
     <row r="36" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="4">
@@ -1227,12 +1272,12 @@
         <v>67</v>
       </c>
       <c r="Q36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R36" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="S36" s="12"/>
+      <c r="S36" s="10"/>
     </row>
     <row r="37" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C37" s="4">
@@ -1248,7 +1293,7 @@
         <v>29</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H37" t="s">
         <v>14</v>
@@ -1280,12 +1325,12 @@
         <v>53</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S37" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="S37" s="10"/>
     </row>
     <row r="38" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C38" s="4">
@@ -1301,7 +1346,7 @@
         <v>30</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>14</v>
@@ -1333,12 +1378,12 @@
         <v>53</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S38" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="S38" s="10"/>
     </row>
     <row r="39" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C39" s="4">
@@ -1354,7 +1399,7 @@
         <v>31</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
@@ -1386,12 +1431,12 @@
         <v>53</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S39" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="S39" s="10"/>
     </row>
     <row r="40" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C40" s="4">
@@ -1407,7 +1452,7 @@
         <v>32</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H40" t="s">
         <v>19</v>
@@ -1436,12 +1481,12 @@
         <v>53</v>
       </c>
       <c r="Q40" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R40" t="s">
         <v>69</v>
       </c>
-      <c r="R40" t="s">
-        <v>72</v>
-      </c>
-      <c r="S40" s="12"/>
+      <c r="S40" s="10"/>
     </row>
     <row r="41" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C41" s="4">
@@ -1457,7 +1502,7 @@
         <v>33</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>19</v>
@@ -1486,12 +1531,12 @@
         <v>53</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="R41" t="s">
-        <v>75</v>
-      </c>
-      <c r="S41" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="S41" s="10"/>
     </row>
     <row r="42" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C42" s="4">
@@ -1536,22 +1581,22 @@
         <v>53</v>
       </c>
       <c r="Q42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R42" t="s">
         <v>69</v>
       </c>
-      <c r="R42" t="s">
-        <v>72</v>
-      </c>
-      <c r="S42" s="12"/>
+      <c r="S42" s="10"/>
     </row>
     <row r="43" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
-      <c r="S43" s="12"/>
+      <c r="S43" s="10"/>
     </row>
     <row r="44" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="S44" s="12"/>
+      <c r="S44" s="10"/>
     </row>
     <row r="45" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C45" s="8">
@@ -1581,7 +1626,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C49" s="8">
         <f>SUMPRODUCT(E40:E42,L40:L42,M40:M42)</f>
         <v>243.20919399838803</v>
@@ -1589,6 +1634,207 @@
       <c r="D49" s="1" t="s">
         <v>63</v>
       </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" t="s">
+        <v>85</v>
+      </c>
+      <c r="E54" t="s">
+        <v>86</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>3.3</v>
+      </c>
+      <c r="E56">
+        <v>0.13</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" s="1">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <v>4.5</v>
+      </c>
+      <c r="E57">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C58" s="1">
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <v>5</v>
+      </c>
+      <c r="E58">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C59" s="1">
+        <v>5</v>
+      </c>
+      <c r="D59">
+        <v>6.5</v>
+      </c>
+      <c r="E59">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C60" s="1">
+        <v>6</v>
+      </c>
+      <c r="D60">
+        <v>8</v>
+      </c>
+      <c r="E60">
+        <v>0.315</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C61" s="1">
+        <v>7</v>
+      </c>
+      <c r="D61">
+        <v>10.3</v>
+      </c>
+      <c r="E61">
+        <v>0.40600000000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C62" s="1">
+        <v>8</v>
+      </c>
+      <c r="D62">
+        <v>12.7</v>
+      </c>
+      <c r="E62">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C63" s="1">
+        <v>9</v>
+      </c>
+      <c r="D63">
+        <v>23</v>
+      </c>
+      <c r="E63">
+        <v>0.94499999999999995</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="1">
+        <v>10</v>
+      </c>
+      <c r="D64">
+        <v>25.4</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C65" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C66" s="1">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s">
+        <v>88</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C67" s="1">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>4</v>
+      </c>
+      <c r="E67" t="s">
+        <v>89</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C71" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
major edit for cost reduction
</commit_message>
<xml_diff>
--- a/export/SM_BOM.xlsx
+++ b/export/SM_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="106">
   <si>
     <t>Item #</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Steel</t>
   </si>
   <si>
-    <t>Deburr</t>
-  </si>
-  <si>
     <t>drawer_support</t>
   </si>
   <si>
@@ -216,12 +213,6 @@
     <t>1.0</t>
   </si>
   <si>
-    <t>Preplated</t>
-  </si>
-  <si>
-    <t>TBD, assume none</t>
-  </si>
-  <si>
     <t>edit</t>
   </si>
   <si>
@@ -292,16 +283,75 @@
   </si>
   <si>
     <t>M4 screw slot</t>
+  </si>
+  <si>
+    <t>Preplate</t>
+  </si>
+  <si>
+    <t>TBD, clear anodize</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>bends</t>
+  </si>
+  <si>
+    <t>per bend</t>
+  </si>
+  <si>
+    <t>al per sqin</t>
+  </si>
+  <si>
+    <t>labor</t>
+  </si>
+  <si>
+    <t>cutting and welding</t>
+  </si>
+  <si>
+    <t>bend cost</t>
+  </si>
+  <si>
+    <t>sqin</t>
+  </si>
+  <si>
+    <t>cutting per in</t>
+  </si>
+  <si>
+    <t>cutting cost</t>
+  </si>
+  <si>
+    <t>sheet metal</t>
+  </si>
+  <si>
+    <t>sm material</t>
+  </si>
+  <si>
+    <t>thermalform total</t>
+  </si>
+  <si>
+    <t>thermalform</t>
+  </si>
+  <si>
+    <t>quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,10 +377,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -358,9 +409,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -659,10 +713,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:S71"/>
+  <dimension ref="C1:AH71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3825" topLeftCell="Q1" activePane="topRight"/>
+      <selection activeCell="C36" sqref="C36"/>
+      <selection pane="topRight" activeCell="AC44" sqref="AC44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,27 +735,42 @@
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
     <col min="17" max="17" width="35" customWidth="1"/>
     <col min="18" max="18" width="41.85546875" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="1"/>
+    <col min="25" max="25" width="13.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8" style="1" customWidth="1"/>
+    <col min="28" max="28" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" customWidth="1"/>
+    <col min="34" max="34" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -711,10 +782,10 @@
     </row>
     <row r="6" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -726,10 +797,10 @@
     </row>
     <row r="7" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -741,10 +812,10 @@
     </row>
     <row r="8" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -786,15 +857,15 @@
     </row>
     <row r="15" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -804,27 +875,27 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -833,85 +904,138 @@
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
-    </row>
-    <row r="21" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T20" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T21" s="13">
+        <f>129/4/10/12/12</f>
+        <v>2.2395833333333334E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="1" t="s">
+    <row r="23" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T23" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T24" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="3:33" x14ac:dyDescent="0.25">
       <c r="J28" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K28" s="11"/>
       <c r="L28" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M28" s="11"/>
     </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="L29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="N29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="R29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="U29" t="s">
+        <v>101</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="X29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C30" s="4">
         <v>1</v>
       </c>
@@ -922,16 +1046,16 @@
         <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H30" t="s">
         <v>10</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J30" s="3">
         <v>194.48</v>
@@ -948,23 +1072,75 @@
         <v>11.593700787401577</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O30" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P30" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R30" t="s">
         <v>67</v>
       </c>
-      <c r="Q30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R30" t="s">
-        <v>70</v>
-      </c>
-      <c r="S30" s="10"/>
-    </row>
-    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T30" s="8">
+        <f>L30*M30</f>
+        <v>88.769406658813338</v>
+      </c>
+      <c r="U30" s="10">
+        <v>9.1</v>
+      </c>
+      <c r="V30" s="10">
+        <f>T30/$T$43*$T$24</f>
+        <v>5.5380383505622843</v>
+      </c>
+      <c r="W30" s="10">
+        <f>T30*$T$21</f>
+        <v>1.9880648366296738</v>
+      </c>
+      <c r="X30" s="10">
+        <f>U30-W30</f>
+        <v>7.1119351633703261</v>
+      </c>
+      <c r="Y30" s="10">
+        <f>X30/((L30+M30)*2)</f>
+        <v>0.18472181073053648</v>
+      </c>
+      <c r="Z30" s="10">
+        <f>(L30+M30)*2*$Y$43</f>
+        <v>2.6338407722565127</v>
+      </c>
+      <c r="AA30" s="8">
+        <v>12</v>
+      </c>
+      <c r="AB30" s="10">
+        <f>X30/AA30</f>
+        <v>0.5926612636141938</v>
+      </c>
+      <c r="AC30" s="10">
+        <f>AA30*$AB$43</f>
+        <v>4.9019776973928941</v>
+      </c>
+      <c r="AD30" s="10">
+        <f>X30-AC30</f>
+        <v>2.2099574659774319</v>
+      </c>
+      <c r="AE30" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF30" s="10">
+        <f>U30</f>
+        <v>9.1</v>
+      </c>
+      <c r="AG30" s="14">
+        <f>AC30/U30</f>
+        <v>0.538678867845373</v>
+      </c>
+    </row>
+    <row r="31" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C31" s="4">
         <v>2</v>
       </c>
@@ -975,16 +1151,16 @@
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J31" s="3">
         <v>464.48</v>
@@ -1001,23 +1177,75 @@
         <v>8.1385826771653544</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S31" s="10"/>
-    </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T31" s="8">
+        <f>L31*M31</f>
+        <v>148.82712133424269</v>
+      </c>
+      <c r="U31" s="10">
+        <v>9.67</v>
+      </c>
+      <c r="V31" s="10">
+        <f>T31/$T$43*$T$24</f>
+        <v>9.284846396694844</v>
+      </c>
+      <c r="W31" s="10">
+        <f>T31*$T$21</f>
+        <v>3.3331074048814768</v>
+      </c>
+      <c r="X31" s="10">
+        <f>U31-W31</f>
+        <v>6.3368925951185231</v>
+      </c>
+      <c r="Y31" s="10">
+        <f t="shared" ref="Y31:Y42" si="1">X31/((L31+M31)*2)</f>
+        <v>0.11990246716031769</v>
+      </c>
+      <c r="Z31" s="10">
+        <f t="shared" ref="Z31:Z42" si="2">(L31+M31)*2*$Y$43</f>
+        <v>3.6154980496125884</v>
+      </c>
+      <c r="AA31" s="8">
+        <v>7</v>
+      </c>
+      <c r="AB31" s="10">
+        <f>X31/AA31</f>
+        <v>0.90527037073121763</v>
+      </c>
+      <c r="AC31" s="10">
+        <f>AA31*$AB$43</f>
+        <v>2.8594869901458551</v>
+      </c>
+      <c r="AD31" s="10">
+        <f>X31-AC31</f>
+        <v>3.477405604972668</v>
+      </c>
+      <c r="AE31" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF31" s="10">
+        <f>U31</f>
+        <v>9.67</v>
+      </c>
+      <c r="AG31" s="14">
+        <f t="shared" ref="AG31:AG42" si="3">AC31/U31</f>
+        <v>0.29570703103886814</v>
+      </c>
+    </row>
+    <row r="32" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C32" s="4">
         <v>3</v>
       </c>
@@ -1028,16 +1256,16 @@
         <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J32" s="3">
         <v>360.65</v>
@@ -1054,23 +1282,75 @@
         <v>16.749212598425199</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S32" s="10"/>
-    </row>
-    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T32" s="8">
+        <f>L32*M32</f>
+        <v>237.81903636307274</v>
+      </c>
+      <c r="U32" s="10">
+        <v>11.26</v>
+      </c>
+      <c r="V32" s="10">
+        <f>T32/$T$43*$T$24</f>
+        <v>14.836766330258014</v>
+      </c>
+      <c r="W32" s="10">
+        <f>T32*$T$21</f>
+        <v>5.3261555018813169</v>
+      </c>
+      <c r="X32" s="10">
+        <f>U32-W32</f>
+        <v>5.9338444981186829</v>
+      </c>
+      <c r="Y32" s="10">
+        <f t="shared" si="1"/>
+        <v>9.5867882564252063E-2</v>
+      </c>
+      <c r="Z32" s="10">
+        <f t="shared" si="2"/>
+        <v>4.2343127336702375</v>
+      </c>
+      <c r="AA32" s="8">
+        <v>5</v>
+      </c>
+      <c r="AB32" s="10">
+        <f>X32/AA32</f>
+        <v>1.1867688996237367</v>
+      </c>
+      <c r="AC32" s="10">
+        <f>AA32*$AB$43</f>
+        <v>2.0424907072470395</v>
+      </c>
+      <c r="AD32" s="10">
+        <f>X32-AC32</f>
+        <v>3.8913537908716433</v>
+      </c>
+      <c r="AE32" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF32" s="10">
+        <f t="shared" ref="AF32:AF37" si="4">U32</f>
+        <v>11.26</v>
+      </c>
+      <c r="AG32" s="14">
+        <f t="shared" si="3"/>
+        <v>0.18139349087451506</v>
+      </c>
+    </row>
+    <row r="33" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C33" s="4">
         <v>4</v>
       </c>
@@ -1081,16 +1361,16 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J33" s="9">
         <v>360.65</v>
@@ -1107,23 +1387,75 @@
         <v>16.749212598425199</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S33" s="10"/>
-    </row>
-    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T33" s="8">
+        <f>L33*M33</f>
+        <v>237.81903636307274</v>
+      </c>
+      <c r="U33" s="10">
+        <v>11.31</v>
+      </c>
+      <c r="V33" s="10">
+        <f>T33/$T$43*$T$24</f>
+        <v>14.836766330258014</v>
+      </c>
+      <c r="W33" s="10">
+        <f>T33*$T$21</f>
+        <v>5.3261555018813169</v>
+      </c>
+      <c r="X33" s="10">
+        <f>U33-W33</f>
+        <v>5.9838444981186836</v>
+      </c>
+      <c r="Y33" s="10">
+        <f t="shared" si="1"/>
+        <v>9.6675688385542538E-2</v>
+      </c>
+      <c r="Z33" s="10">
+        <f t="shared" si="2"/>
+        <v>4.2343127336702375</v>
+      </c>
+      <c r="AA33" s="8">
+        <v>5</v>
+      </c>
+      <c r="AB33" s="10">
+        <f>X33/AA33</f>
+        <v>1.1967688996237367</v>
+      </c>
+      <c r="AC33" s="10">
+        <f>AA33*$AB$43</f>
+        <v>2.0424907072470395</v>
+      </c>
+      <c r="AD33" s="10">
+        <f>X33-AC33</f>
+        <v>3.9413537908716441</v>
+      </c>
+      <c r="AE33" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF33" s="10">
+        <f t="shared" si="4"/>
+        <v>11.31</v>
+      </c>
+      <c r="AG33" s="14">
+        <f t="shared" si="3"/>
+        <v>0.18059157446923427</v>
+      </c>
+    </row>
+    <row r="34" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C34" s="4">
         <v>5</v>
       </c>
@@ -1134,16 +1466,16 @@
         <v>2</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J34" s="3">
         <v>704.42</v>
@@ -1160,23 +1492,75 @@
         <v>17.238582677165354</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R34" t="s">
-        <v>71</v>
-      </c>
-      <c r="S34" s="10"/>
-    </row>
-    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="T34" s="8">
+        <f>L34*M34</f>
+        <v>478.07883501766997</v>
+      </c>
+      <c r="U34" s="10">
+        <v>16.86</v>
+      </c>
+      <c r="V34" s="10">
+        <f>T34/$T$43*$T$24</f>
+        <v>29.825803985557346</v>
+      </c>
+      <c r="W34" s="10">
+        <f>T34*$T$21</f>
+        <v>10.7069739092499</v>
+      </c>
+      <c r="X34" s="10">
+        <f>U34-W34</f>
+        <v>6.1530260907500995</v>
+      </c>
+      <c r="Y34" s="10">
+        <f t="shared" si="1"/>
+        <v>6.8410049508462259E-2</v>
+      </c>
+      <c r="Z34" s="10">
+        <f t="shared" si="2"/>
+        <v>6.1530260907500995</v>
+      </c>
+      <c r="AA34" s="8">
+        <v>3</v>
+      </c>
+      <c r="AB34" s="10">
+        <f>X34/AA34</f>
+        <v>2.0510086969166998</v>
+      </c>
+      <c r="AC34" s="10">
+        <f>AA34*$AB$43</f>
+        <v>1.2254944243482235</v>
+      </c>
+      <c r="AD34" s="10">
+        <f>X34-AC34</f>
+        <v>4.927531666401876</v>
+      </c>
+      <c r="AE34" s="8">
+        <v>2</v>
+      </c>
+      <c r="AF34" s="10">
+        <f t="shared" si="4"/>
+        <v>16.86</v>
+      </c>
+      <c r="AG34" s="14">
+        <f t="shared" si="3"/>
+        <v>7.268650203726118E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C35" s="4">
         <v>6</v>
       </c>
@@ -1187,16 +1571,16 @@
         <v>2</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J35" s="3">
         <v>323.14</v>
@@ -1213,40 +1597,92 @@
         <v>12.722047244094489</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="Q35" t="s">
-        <v>74</v>
-      </c>
-      <c r="S35" s="10"/>
-    </row>
-    <row r="36" spans="3:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="T35" s="8">
+        <f>L35*M35</f>
+        <v>161.85048608097216</v>
+      </c>
+      <c r="U35" s="10">
+        <v>38.57</v>
+      </c>
+      <c r="V35" s="10">
+        <f>T35/$T$43*$T$24</f>
+        <v>10.097332321017378</v>
+      </c>
+      <c r="W35" s="10">
+        <f>T35*$T$21</f>
+        <v>3.6247765111884389</v>
+      </c>
+      <c r="X35" s="10">
+        <f>U35-W35</f>
+        <v>34.945223488811564</v>
+      </c>
+      <c r="Y35" s="10">
+        <f t="shared" si="1"/>
+        <v>0.68670597621449969</v>
+      </c>
+      <c r="Z35" s="10">
+        <f t="shared" si="2"/>
+        <v>3.481263527269999</v>
+      </c>
+      <c r="AA35" s="8">
+        <v>8</v>
+      </c>
+      <c r="AB35" s="10">
+        <f>X35/AA35</f>
+        <v>4.3681529361014455</v>
+      </c>
+      <c r="AC35" s="10">
+        <f>AA35*$AB$43</f>
+        <v>3.267985131595263</v>
+      </c>
+      <c r="AD35" s="10">
+        <f>X35-AC35</f>
+        <v>31.6772383572163</v>
+      </c>
+      <c r="AE35" s="8">
+        <v>2</v>
+      </c>
+      <c r="AF35" s="10">
+        <f>MIN(U35:V35)</f>
+        <v>10.097332321017378</v>
+      </c>
+      <c r="AG35" s="14">
+        <f t="shared" si="3"/>
+        <v>8.4728678547971559E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="4">
         <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E36" s="4">
         <v>1</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J36" s="3">
         <v>251</v>
@@ -1263,23 +1699,75 @@
         <v>11.618110236220474</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="S36" s="10"/>
-    </row>
-    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="T36" s="8">
+        <f>L36*M36</f>
+        <v>114.80888461776925</v>
+      </c>
+      <c r="U36" s="10">
+        <v>6.13</v>
+      </c>
+      <c r="V36" s="10">
+        <f>T36/$T$43*$T$24</f>
+        <v>7.1625577992455849</v>
+      </c>
+      <c r="W36" s="10">
+        <f>T36*$T$21</f>
+        <v>2.571240645085457</v>
+      </c>
+      <c r="X36" s="10">
+        <f>U36-W36</f>
+        <v>3.5587593549145429</v>
+      </c>
+      <c r="Y36" s="10">
+        <f t="shared" si="1"/>
+        <v>8.2761845463128911E-2</v>
+      </c>
+      <c r="Z36" s="10">
+        <f t="shared" si="2"/>
+        <v>2.9416321288638771</v>
+      </c>
+      <c r="AA36" s="8">
+        <v>6</v>
+      </c>
+      <c r="AB36" s="10">
+        <f>X36/AA36</f>
+        <v>0.59312655915242385</v>
+      </c>
+      <c r="AC36" s="10">
+        <f>AA36*$AB$43</f>
+        <v>2.4509888486964471</v>
+      </c>
+      <c r="AD36" s="10">
+        <f>X36-AC36</f>
+        <v>1.1077705062180958</v>
+      </c>
+      <c r="AE36" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF36" s="10">
+        <f t="shared" si="4"/>
+        <v>6.13</v>
+      </c>
+      <c r="AG36" s="14">
+        <f t="shared" si="3"/>
+        <v>0.39983504872698972</v>
+      </c>
+    </row>
+    <row r="37" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C37" s="4">
         <v>8</v>
       </c>
@@ -1290,16 +1778,16 @@
         <v>1</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H37" t="s">
         <v>14</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="J37" s="3">
         <v>350</v>
@@ -1316,23 +1804,75 @@
         <v>10.60944881889764</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="O37" t="s">
-        <v>15</v>
+        <v>54</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="P37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S37" s="10"/>
-    </row>
-    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="T37" s="8">
+        <f>L37*M37</f>
+        <v>146.19319238638479</v>
+      </c>
+      <c r="U37" s="10">
+        <v>12.37</v>
+      </c>
+      <c r="V37" s="10">
+        <f>T37/$T$43*$T$24</f>
+        <v>9.1205240239886969</v>
+      </c>
+      <c r="W37" s="10">
+        <f>T37*$T$21</f>
+        <v>3.2741183711534094</v>
+      </c>
+      <c r="X37" s="10">
+        <f>U37-W37</f>
+        <v>9.0958816288465894</v>
+      </c>
+      <c r="Y37" s="10">
+        <f t="shared" si="1"/>
+        <v>0.18647526423185845</v>
+      </c>
+      <c r="Z37" s="10">
+        <f t="shared" si="2"/>
+        <v>3.3369021629529296</v>
+      </c>
+      <c r="AA37" s="8">
+        <v>13</v>
+      </c>
+      <c r="AB37" s="10">
+        <f>X37/AA37</f>
+        <v>0.6996832022189684</v>
+      </c>
+      <c r="AC37" s="10">
+        <f>AA37*$AB$43</f>
+        <v>5.3104758388423026</v>
+      </c>
+      <c r="AD37" s="10">
+        <f>X37-AC37</f>
+        <v>3.7854057900042868</v>
+      </c>
+      <c r="AE37" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF37" s="10">
+        <f t="shared" si="4"/>
+        <v>12.37</v>
+      </c>
+      <c r="AG37" s="14">
+        <f t="shared" si="3"/>
+        <v>0.42930281639792262</v>
+      </c>
+    </row>
+    <row r="38" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C38" s="4">
         <v>9</v>
       </c>
@@ -1343,16 +1883,16 @@
         <v>1</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="J38" s="3">
         <v>1201.6600000000001</v>
@@ -1369,23 +1909,72 @@
         <v>8.1893700787401578</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S38" s="10"/>
-    </row>
-    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="T38" s="8">
+        <f>L38*M38</f>
+        <v>387.43458459916923</v>
+      </c>
+      <c r="U38" s="10">
+        <v>21.55</v>
+      </c>
+      <c r="V38" s="10">
+        <f>T38/$T$43*$T$24</f>
+        <v>24.170800150677156</v>
+      </c>
+      <c r="W38" s="10">
+        <f>T38*$T$21</f>
+        <v>8.6769203842522273</v>
+      </c>
+      <c r="X38" s="10">
+        <f>U38-W38</f>
+        <v>12.873079615747773</v>
+      </c>
+      <c r="Y38" s="10">
+        <f t="shared" si="1"/>
+        <v>0.11597615833492711</v>
+      </c>
+      <c r="Z38" s="10">
+        <f t="shared" si="2"/>
+        <v>7.5933538968971659</v>
+      </c>
+      <c r="AA38" s="8">
+        <v>16</v>
+      </c>
+      <c r="AB38" s="10">
+        <f>X38/AA38</f>
+        <v>0.80456747598423584</v>
+      </c>
+      <c r="AC38" s="10">
+        <f>AA38*$AB$43</f>
+        <v>6.5359702631905261</v>
+      </c>
+      <c r="AD38" s="10">
+        <f>X38-AC38</f>
+        <v>6.3371093525572473</v>
+      </c>
+      <c r="AE38" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="14">
+        <f t="shared" si="3"/>
+        <v>0.3032932836747344</v>
+      </c>
+    </row>
+    <row r="39" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C39" s="4">
         <v>10</v>
       </c>
@@ -1396,16 +1985,16 @@
         <v>1</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="J39" s="3">
         <v>981.66</v>
@@ -1422,40 +2011,89 @@
         <v>8.30748031496063</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S39" s="10"/>
-    </row>
-    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="T39" s="8">
+        <f>L39*M39</f>
+        <v>321.06776086552173</v>
+      </c>
+      <c r="U39" s="10">
+        <v>22.24</v>
+      </c>
+      <c r="V39" s="10">
+        <f>T39/$T$43*$T$24</f>
+        <v>20.030387041298145</v>
+      </c>
+      <c r="W39" s="10">
+        <f>T39*$T$21</f>
+        <v>7.1905800610507473</v>
+      </c>
+      <c r="X39" s="10">
+        <f>U39-W39</f>
+        <v>15.049419938949251</v>
+      </c>
+      <c r="Y39" s="10">
+        <f t="shared" si="1"/>
+        <v>0.16025189970792886</v>
+      </c>
+      <c r="Z39" s="10">
+        <f t="shared" si="2"/>
+        <v>6.4244577753746199</v>
+      </c>
+      <c r="AA39" s="8">
+        <v>18</v>
+      </c>
+      <c r="AB39" s="10">
+        <f>X39/AA39</f>
+        <v>0.83607888549718057</v>
+      </c>
+      <c r="AC39" s="10">
+        <f>AA39*$AB$43</f>
+        <v>7.3529665460893421</v>
+      </c>
+      <c r="AD39" s="10">
+        <f>X39-AC39</f>
+        <v>7.696453392859909</v>
+      </c>
+      <c r="AE39" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF39" s="10"/>
+      <c r="AG39" s="14">
+        <f t="shared" si="3"/>
+        <v>0.33061899937452083</v>
+      </c>
+    </row>
+    <row r="40" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C40" s="4">
         <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E40" s="4">
         <v>2</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J40" s="3">
         <v>331.78</v>
@@ -1472,40 +2110,92 @@
         <v>8.5161417322834652</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R40" t="s">
-        <v>69</v>
-      </c>
-      <c r="S40" s="10"/>
-    </row>
-    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="T40" s="8">
+        <f>L40*M40</f>
+        <v>111.23958676917356</v>
+      </c>
+      <c r="U40" s="10">
+        <v>6.55</v>
+      </c>
+      <c r="V40" s="10">
+        <f>T40/$T$43*$T$24</f>
+        <v>6.9398807631572756</v>
+      </c>
+      <c r="W40" s="10">
+        <f>T40*$T$21</f>
+        <v>2.4913032453512827</v>
+      </c>
+      <c r="X40" s="10">
+        <f>U40-W40</f>
+        <v>4.0586967546487172</v>
+      </c>
+      <c r="Y40" s="10">
+        <f t="shared" si="1"/>
+        <v>9.4045592483056994E-2</v>
+      </c>
+      <c r="Z40" s="10">
+        <f t="shared" si="2"/>
+        <v>2.9523514988262267</v>
+      </c>
+      <c r="AA40" s="8">
+        <v>7</v>
+      </c>
+      <c r="AB40" s="10">
+        <f>X40/AA40</f>
+        <v>0.57981382209267385</v>
+      </c>
+      <c r="AC40" s="10">
+        <f>AA40*$AB$43</f>
+        <v>2.8594869901458551</v>
+      </c>
+      <c r="AD40" s="10">
+        <f>X40-AC40</f>
+        <v>1.1992097645028621</v>
+      </c>
+      <c r="AE40" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF40" s="10">
+        <f t="shared" ref="AF40:AF42" si="5">U40</f>
+        <v>6.55</v>
+      </c>
+      <c r="AG40" s="14">
+        <f t="shared" si="3"/>
+        <v>0.43656289925890918</v>
+      </c>
+    </row>
+    <row r="41" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C41" s="4">
         <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E41" s="4">
         <v>2</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J41" s="3">
         <v>30</v>
@@ -1522,40 +2212,92 @@
         <v>3.6295275590551181</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R41" t="s">
-        <v>72</v>
-      </c>
-      <c r="S41" s="10"/>
-    </row>
-    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="T41" s="8">
+        <f>L41*M41</f>
+        <v>4.2868435736871477</v>
+      </c>
+      <c r="U41" s="10">
+        <v>1.73</v>
+      </c>
+      <c r="V41" s="10">
+        <f>T41/$T$43*$T$24</f>
+        <v>0.26744241070787694</v>
+      </c>
+      <c r="W41" s="10">
+        <f>T41*$T$21</f>
+        <v>9.6007434202368416E-2</v>
+      </c>
+      <c r="X41" s="10">
+        <f>U41-W41</f>
+        <v>1.6339925657976315</v>
+      </c>
+      <c r="Y41" s="10">
+        <f t="shared" si="1"/>
+        <v>0.16983145581168607</v>
+      </c>
+      <c r="Z41" s="10">
+        <f t="shared" si="2"/>
+        <v>0.65819086216055145</v>
+      </c>
+      <c r="AA41" s="8">
+        <v>4</v>
+      </c>
+      <c r="AB41" s="10">
+        <f>X41/AA41</f>
+        <v>0.40849814144940788</v>
+      </c>
+      <c r="AC41" s="10">
+        <f>AA41*$AB$43</f>
+        <v>1.6339925657976315</v>
+      </c>
+      <c r="AD41" s="10">
+        <f>X41-AC41</f>
+        <v>0</v>
+      </c>
+      <c r="AE41" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF41" s="10">
+        <f t="shared" si="5"/>
+        <v>1.73</v>
+      </c>
+      <c r="AG41" s="14">
+        <f t="shared" si="3"/>
+        <v>0.94450437329342862</v>
+      </c>
+    </row>
+    <row r="42" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C42" s="4">
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E42" s="4">
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J42" s="3">
         <v>66</v>
@@ -1572,58 +2314,161 @@
         <v>4.6783464566929132</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R42" t="s">
-        <v>69</v>
-      </c>
-      <c r="S42" s="10"/>
-    </row>
-    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="T42" s="8">
+        <f>L42*M42</f>
+        <v>12.156333312666627</v>
+      </c>
+      <c r="U42" s="10">
+        <v>1.45</v>
+      </c>
+      <c r="V42" s="10">
+        <f>T42/$T$43*$T$24</f>
+        <v>0.75839461613751413</v>
+      </c>
+      <c r="W42" s="10">
+        <f>T42*$T$21</f>
+        <v>0.27225121481492964</v>
+      </c>
+      <c r="X42" s="10">
+        <f>U42-W42</f>
+        <v>1.1777487851850703</v>
+      </c>
+      <c r="Y42" s="10">
+        <f t="shared" si="1"/>
+        <v>8.0925226271981787E-2</v>
+      </c>
+      <c r="Z42" s="10">
+        <f t="shared" si="2"/>
+        <v>0.99560861816134483</v>
+      </c>
+      <c r="AA42" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB42" s="10">
+        <f>X42/AA42</f>
+        <v>1.1777487851850703</v>
+      </c>
+      <c r="AC42" s="10">
+        <f>AA42*$AB$43</f>
+        <v>0.40849814144940788</v>
+      </c>
+      <c r="AD42" s="10">
+        <f>X42-AC42</f>
+        <v>0.76925064373566243</v>
+      </c>
+      <c r="AE42" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF42" s="10">
+        <f t="shared" si="5"/>
+        <v>1.45</v>
+      </c>
+      <c r="AG42" s="14">
+        <f t="shared" si="3"/>
+        <v>0.28172285617200543</v>
+      </c>
+    </row>
+    <row r="43" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
-      <c r="S43" s="10"/>
-    </row>
-    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T43" s="10">
+        <f>SUMPRODUCT(E30:E42,T30:T42)</f>
+        <v>3205.8068593837188</v>
+      </c>
+      <c r="U43" s="10">
+        <f>SUMPRODUCT(E30:E42,U30:U42)</f>
+        <v>232.5</v>
+      </c>
+      <c r="V43" s="10">
+        <f>SUMPRODUCT(E30:E42,V30:V42)</f>
+        <v>200.00000000000003</v>
+      </c>
+      <c r="W43" s="10">
+        <f>T43*$T$21</f>
+        <v>71.796716121614537</v>
+      </c>
+      <c r="X43" s="10"/>
+      <c r="Y43" s="10">
+        <f>MIN(Y30:Y42)</f>
+        <v>6.8410049508462259E-2</v>
+      </c>
+      <c r="Z43" s="10">
+        <f>SUMPRODUCT(Z30:Z42,E30:E42)</f>
+        <v>62.499582829473269</v>
+      </c>
+      <c r="AA43" s="10"/>
+      <c r="AB43" s="10">
+        <f>MIN(AB30:AB42)</f>
+        <v>0.40849814144940788</v>
+      </c>
+      <c r="AC43" s="10">
+        <f>SUMPRODUCT(AC30:AC42,E30:E42)</f>
+        <v>51.879263964074795</v>
+      </c>
+      <c r="AD43" s="10"/>
+      <c r="AE43" s="10"/>
+      <c r="AF43" s="10">
+        <f>SUMPRODUCT(AE30:AE42,AF30:AF42)</f>
+        <v>123.48466464203476</v>
+      </c>
+    </row>
+    <row r="44" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S44" s="10"/>
-    </row>
-    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="T44" s="10"/>
+      <c r="U44" s="10"/>
+      <c r="V44" s="10"/>
+      <c r="W44" s="10"/>
+      <c r="X44" s="10"/>
+      <c r="Y44" s="10"/>
+      <c r="Z44" s="10"/>
+      <c r="AA44" s="10"/>
+      <c r="AB44" s="10"/>
+      <c r="AC44" s="10"/>
+      <c r="AD44" s="10"/>
+      <c r="AE44" s="10"/>
+      <c r="AF44" s="10"/>
+    </row>
+    <row r="45" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C45" s="8">
         <f>SUMPRODUCT(L30:L36,M30:M36,E30:E36)</f>
         <v>2107.9021275342552</v>
       </c>
       <c r="D45" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C47" s="8">
         <f>SUMPRODUCT(M37:M39,L37:L39,E37:E39)</f>
         <v>854.69553785107564</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
@@ -1632,26 +2477,26 @@
         <v>243.20919399838803</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D54" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E54" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
@@ -1665,7 +2510,7 @@
         <v>0.11799999999999999</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
@@ -1679,7 +2524,7 @@
         <v>0.13</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
@@ -1693,7 +2538,7 @@
         <v>0.11700000000000001</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
@@ -1707,7 +2552,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
@@ -1721,7 +2566,7 @@
         <v>0.25700000000000001</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
@@ -1735,7 +2580,7 @@
         <v>0.315</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
@@ -1784,16 +2629,16 @@
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
@@ -1804,10 +2649,10 @@
         <v>3</v>
       </c>
       <c r="E66" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
@@ -1818,10 +2663,10 @@
         <v>4</v>
       </c>
       <c r="E67" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
continue cost reduction improvements
</commit_message>
<xml_diff>
--- a/export/SM_BOM.xlsx
+++ b/export/SM_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="109">
   <si>
     <t>Item #</t>
   </si>
@@ -321,9 +321,6 @@
     <t>cutting cost</t>
   </si>
   <si>
-    <t>sheet metal</t>
-  </si>
-  <si>
     <t>sm material</t>
   </si>
   <si>
@@ -334,6 +331,18 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>sparqtron</t>
+  </si>
+  <si>
+    <t>anodizing</t>
+  </si>
+  <si>
+    <t>finishing</t>
+  </si>
+  <si>
+    <t>RFMI</t>
   </si>
 </sst>
 </file>
@@ -342,7 +351,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -381,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -404,13 +413,16 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,12 +725,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:AH71"/>
+  <dimension ref="C1:AJ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3825" topLeftCell="Q1" activePane="topRight"/>
-      <selection activeCell="C36" sqref="C36"/>
-      <selection pane="topRight" activeCell="AC44" sqref="AC44"/>
+    <sheetView tabSelected="1" topLeftCell="C23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3825" topLeftCell="S1" activePane="topRight"/>
+      <selection activeCell="C29" sqref="C29:D42"/>
+      <selection pane="topRight" activeCell="AB44" sqref="AB44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,19 +750,21 @@
     <col min="19" max="19" width="12" style="1" customWidth="1"/>
     <col min="20" max="20" width="11.7109375" customWidth="1"/>
     <col min="21" max="21" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="1"/>
-    <col min="25" max="25" width="13.42578125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8" style="1" customWidth="1"/>
-    <col min="28" max="28" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.28515625" customWidth="1"/>
-    <col min="34" max="34" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="1"/>
+    <col min="26" max="26" width="13.42578125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8" style="1" customWidth="1"/>
+    <col min="29" max="29" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.5703125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.28515625" customWidth="1"/>
+    <col min="36" max="36" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -769,61 +783,61 @@
       <c r="D5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
     </row>
     <row r="8" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
@@ -864,33 +878,33 @@
       <c r="D16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-    </row>
-    <row r="17" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" spans="3:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
         <v>56</v>
       </c>
@@ -908,45 +922,45 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T21" s="13">
+      <c r="T21" s="12">
         <f>129/4/10/12/12</f>
         <v>2.2395833333333334E-2</v>
       </c>
     </row>
-    <row r="22" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E22" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="3:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T24" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="J28" s="11" t="s">
+    <row r="25" spans="3:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="J28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11" t="s">
+      <c r="K28" s="13"/>
+      <c r="L28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M28" s="11"/>
-    </row>
-    <row r="29" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="M28" s="13"/>
+    </row>
+    <row r="29" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
@@ -999,43 +1013,52 @@
         <v>98</v>
       </c>
       <c r="U29" t="s">
+        <v>108</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="X29" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="V29" s="1" t="s">
+      <c r="Y29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG29" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="W29" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="X29" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y29" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z29" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB29" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC29" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD29" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE29" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF29" t="s">
+      <c r="AH29" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="30" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C30" s="4">
         <v>1</v>
       </c>
@@ -1087,60 +1110,67 @@
         <v>67</v>
       </c>
       <c r="T30" s="8">
-        <f>L30*M30</f>
+        <f t="shared" ref="T30:T42" si="0">L30*M30</f>
         <v>88.769406658813338</v>
       </c>
       <c r="U30" s="10">
         <v>9.1</v>
       </c>
-      <c r="V30" s="10">
-        <f>T30/$T$43*$T$24</f>
+      <c r="V30" s="1">
+        <v>17</v>
+      </c>
+      <c r="W30" s="10">
+        <f t="shared" ref="W30:W42" si="1">T30/$T$43*$T$24</f>
         <v>5.5380383505622843</v>
       </c>
-      <c r="W30" s="10">
-        <f>T30*$T$21</f>
+      <c r="X30" s="10">
+        <f t="shared" ref="X30:X43" si="2">T30*$T$21</f>
         <v>1.9880648366296738</v>
       </c>
-      <c r="X30" s="10">
-        <f>U30-W30</f>
+      <c r="Y30" s="10">
+        <f t="shared" ref="Y30:Y42" si="3">U30-X30</f>
         <v>7.1119351633703261</v>
       </c>
-      <c r="Y30" s="10">
-        <f>X30/((L30+M30)*2)</f>
+      <c r="Z30" s="10">
+        <f>Y30/((L30+M30)*2)</f>
         <v>0.18472181073053648</v>
       </c>
-      <c r="Z30" s="10">
-        <f>(L30+M30)*2*$Y$43</f>
+      <c r="AA30" s="10">
+        <f>(L30+M30)*2*$Z$43</f>
         <v>2.6338407722565127</v>
       </c>
-      <c r="AA30" s="8">
+      <c r="AB30" s="8">
         <v>12</v>
       </c>
-      <c r="AB30" s="10">
-        <f>X30/AA30</f>
+      <c r="AC30" s="10">
+        <f t="shared" ref="AC30:AC42" si="4">Y30/AB30</f>
         <v>0.5926612636141938</v>
       </c>
-      <c r="AC30" s="10">
-        <f>AA30*$AB$43</f>
+      <c r="AD30" s="10">
+        <f t="shared" ref="AD30:AD42" si="5">AB30*$AC$43</f>
         <v>4.9019776973928941</v>
       </c>
-      <c r="AD30" s="10">
-        <f>X30-AC30</f>
+      <c r="AE30" s="10">
+        <f t="shared" ref="AE30:AE42" si="6">Y30-AD30</f>
         <v>2.2099574659774319</v>
       </c>
-      <c r="AE30" s="8">
+      <c r="AF30" s="10">
+        <f>(V30-U30)/T30</f>
+        <v>8.8994624357057822E-2</v>
+      </c>
+      <c r="AG30" s="8">
         <v>1</v>
       </c>
-      <c r="AF30" s="10">
+      <c r="AH30" s="10">
         <f>U30</f>
         <v>9.1</v>
       </c>
-      <c r="AG30" s="14">
-        <f>AC30/U30</f>
-        <v>0.538678867845373</v>
-      </c>
-    </row>
-    <row r="31" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI30" s="15">
+        <f>0.5*T30</f>
+        <v>44.384703329406669</v>
+      </c>
+    </row>
+    <row r="31" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C31" s="4">
         <v>2</v>
       </c>
@@ -1169,11 +1199,11 @@
         <v>206.72</v>
       </c>
       <c r="L31" s="5">
-        <f t="shared" ref="L31:M42" si="0">J31/25.4</f>
+        <f t="shared" ref="L31:M42" si="7">J31/25.4</f>
         <v>18.286614173228347</v>
       </c>
       <c r="M31" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8.1385826771653544</v>
       </c>
       <c r="N31" s="6" t="s">
@@ -1192,60 +1222,67 @@
         <v>67</v>
       </c>
       <c r="T31" s="8">
-        <f>L31*M31</f>
+        <f t="shared" si="0"/>
         <v>148.82712133424269</v>
       </c>
       <c r="U31" s="10">
         <v>9.67</v>
       </c>
-      <c r="V31" s="10">
-        <f>T31/$T$43*$T$24</f>
+      <c r="V31" s="1">
+        <v>18</v>
+      </c>
+      <c r="W31" s="10">
+        <f t="shared" si="1"/>
         <v>9.284846396694844</v>
       </c>
-      <c r="W31" s="10">
-        <f>T31*$T$21</f>
+      <c r="X31" s="10">
+        <f t="shared" si="2"/>
         <v>3.3331074048814768</v>
       </c>
-      <c r="X31" s="10">
-        <f>U31-W31</f>
+      <c r="Y31" s="10">
+        <f t="shared" si="3"/>
         <v>6.3368925951185231</v>
       </c>
-      <c r="Y31" s="10">
-        <f t="shared" ref="Y31:Y42" si="1">X31/((L31+M31)*2)</f>
+      <c r="Z31" s="10">
+        <f t="shared" ref="Z31:Z42" si="8">Y31/((L31+M31)*2)</f>
         <v>0.11990246716031769</v>
       </c>
-      <c r="Z31" s="10">
-        <f t="shared" ref="Z31:Z42" si="2">(L31+M31)*2*$Y$43</f>
+      <c r="AA31" s="10">
+        <f t="shared" ref="AA31:AA42" si="9">(L31+M31)*2*$Z$43</f>
         <v>3.6154980496125884</v>
       </c>
-      <c r="AA31" s="8">
+      <c r="AB31" s="8">
         <v>7</v>
       </c>
-      <c r="AB31" s="10">
-        <f>X31/AA31</f>
+      <c r="AC31" s="10">
+        <f t="shared" si="4"/>
         <v>0.90527037073121763</v>
       </c>
-      <c r="AC31" s="10">
-        <f>AA31*$AB$43</f>
+      <c r="AD31" s="10">
+        <f t="shared" si="5"/>
         <v>2.8594869901458551</v>
       </c>
-      <c r="AD31" s="10">
-        <f>X31-AC31</f>
+      <c r="AE31" s="10">
+        <f t="shared" si="6"/>
         <v>3.477405604972668</v>
       </c>
-      <c r="AE31" s="8">
+      <c r="AF31" s="10">
+        <f t="shared" ref="AF31:AF42" si="10">(V31-U31)/T31</f>
+        <v>5.5970981131134752E-2</v>
+      </c>
+      <c r="AG31" s="8">
         <v>1</v>
       </c>
-      <c r="AF31" s="10">
+      <c r="AH31" s="10">
         <f>U31</f>
         <v>9.67</v>
       </c>
-      <c r="AG31" s="14">
-        <f t="shared" ref="AG31:AG42" si="3">AC31/U31</f>
-        <v>0.29570703103886814</v>
-      </c>
-    </row>
-    <row r="32" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI31" s="15">
+        <f t="shared" ref="AI31:AI42" si="11">0.5*T31</f>
+        <v>74.413560667121345</v>
+      </c>
+    </row>
+    <row r="32" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C32" s="4">
         <v>3</v>
       </c>
@@ -1274,11 +1311,11 @@
         <v>425.43</v>
       </c>
       <c r="L32" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>14.198818897637794</v>
       </c>
       <c r="M32" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>16.749212598425199</v>
       </c>
       <c r="N32" s="6" t="s">
@@ -1297,60 +1334,67 @@
         <v>67</v>
       </c>
       <c r="T32" s="8">
-        <f>L32*M32</f>
+        <f t="shared" si="0"/>
         <v>237.81903636307274</v>
       </c>
       <c r="U32" s="10">
         <v>11.26</v>
       </c>
-      <c r="V32" s="10">
-        <f>T32/$T$43*$T$24</f>
+      <c r="V32" s="1">
+        <v>29</v>
+      </c>
+      <c r="W32" s="10">
+        <f t="shared" si="1"/>
         <v>14.836766330258014</v>
       </c>
-      <c r="W32" s="10">
-        <f>T32*$T$21</f>
+      <c r="X32" s="10">
+        <f t="shared" si="2"/>
         <v>5.3261555018813169</v>
       </c>
-      <c r="X32" s="10">
-        <f>U32-W32</f>
+      <c r="Y32" s="10">
+        <f t="shared" si="3"/>
         <v>5.9338444981186829</v>
       </c>
-      <c r="Y32" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z32" s="10">
+        <f t="shared" si="8"/>
         <v>9.5867882564252063E-2</v>
       </c>
-      <c r="Z32" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA32" s="10">
+        <f t="shared" si="9"/>
         <v>4.2343127336702375</v>
       </c>
-      <c r="AA32" s="8">
+      <c r="AB32" s="8">
         <v>5</v>
       </c>
-      <c r="AB32" s="10">
-        <f>X32/AA32</f>
+      <c r="AC32" s="10">
+        <f t="shared" si="4"/>
         <v>1.1867688996237367</v>
       </c>
-      <c r="AC32" s="10">
-        <f>AA32*$AB$43</f>
+      <c r="AD32" s="10">
+        <f t="shared" si="5"/>
         <v>2.0424907072470395</v>
       </c>
-      <c r="AD32" s="10">
-        <f>X32-AC32</f>
+      <c r="AE32" s="10">
+        <f t="shared" si="6"/>
         <v>3.8913537908716433</v>
       </c>
-      <c r="AE32" s="8">
+      <c r="AF32" s="10">
+        <f t="shared" si="10"/>
+        <v>7.4594533184958164E-2</v>
+      </c>
+      <c r="AG32" s="8">
         <v>1</v>
       </c>
-      <c r="AF32" s="10">
-        <f t="shared" ref="AF32:AF37" si="4">U32</f>
+      <c r="AH32" s="10">
+        <f t="shared" ref="AH32:AH37" si="12">U32</f>
         <v>11.26</v>
       </c>
-      <c r="AG32" s="14">
-        <f t="shared" si="3"/>
-        <v>0.18139349087451506</v>
-      </c>
-    </row>
-    <row r="33" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI32" s="15">
+        <f t="shared" si="11"/>
+        <v>118.90951818153637</v>
+      </c>
+    </row>
+    <row r="33" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C33" s="4">
         <v>4</v>
       </c>
@@ -1379,11 +1423,11 @@
         <v>425.43</v>
       </c>
       <c r="L33" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>14.198818897637794</v>
       </c>
       <c r="M33" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>16.749212598425199</v>
       </c>
       <c r="N33" s="6" t="s">
@@ -1402,60 +1446,67 @@
         <v>67</v>
       </c>
       <c r="T33" s="8">
-        <f>L33*M33</f>
+        <f t="shared" si="0"/>
         <v>237.81903636307274</v>
       </c>
       <c r="U33" s="10">
         <v>11.31</v>
       </c>
-      <c r="V33" s="10">
-        <f>T33/$T$43*$T$24</f>
+      <c r="V33" s="1">
+        <v>26</v>
+      </c>
+      <c r="W33" s="10">
+        <f t="shared" si="1"/>
         <v>14.836766330258014</v>
       </c>
-      <c r="W33" s="10">
-        <f>T33*$T$21</f>
+      <c r="X33" s="10">
+        <f t="shared" si="2"/>
         <v>5.3261555018813169</v>
       </c>
-      <c r="X33" s="10">
-        <f>U33-W33</f>
+      <c r="Y33" s="10">
+        <f t="shared" si="3"/>
         <v>5.9838444981186836</v>
       </c>
-      <c r="Y33" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z33" s="10">
+        <f t="shared" si="8"/>
         <v>9.6675688385542538E-2</v>
       </c>
-      <c r="Z33" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA33" s="10">
+        <f t="shared" si="9"/>
         <v>4.2343127336702375</v>
       </c>
-      <c r="AA33" s="8">
+      <c r="AB33" s="8">
         <v>5</v>
       </c>
-      <c r="AB33" s="10">
-        <f>X33/AA33</f>
+      <c r="AC33" s="10">
+        <f t="shared" si="4"/>
         <v>1.1967688996237367</v>
       </c>
-      <c r="AC33" s="10">
-        <f>AA33*$AB$43</f>
+      <c r="AD33" s="10">
+        <f t="shared" si="5"/>
         <v>2.0424907072470395</v>
       </c>
-      <c r="AD33" s="10">
-        <f>X33-AC33</f>
+      <c r="AE33" s="10">
+        <f t="shared" si="6"/>
         <v>3.9413537908716441</v>
       </c>
-      <c r="AE33" s="8">
+      <c r="AF33" s="10">
+        <f t="shared" si="10"/>
+        <v>6.1769655720802438E-2</v>
+      </c>
+      <c r="AG33" s="8">
         <v>1</v>
       </c>
-      <c r="AF33" s="10">
-        <f t="shared" si="4"/>
+      <c r="AH33" s="10">
+        <f t="shared" si="12"/>
         <v>11.31</v>
       </c>
-      <c r="AG33" s="14">
-        <f t="shared" si="3"/>
-        <v>0.18059157446923427</v>
-      </c>
-    </row>
-    <row r="34" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI33" s="15">
+        <f t="shared" si="11"/>
+        <v>118.90951818153637</v>
+      </c>
+    </row>
+    <row r="34" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C34" s="4">
         <v>5</v>
       </c>
@@ -1484,11 +1535,11 @@
         <v>437.86</v>
       </c>
       <c r="L34" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>27.73307086614173</v>
       </c>
       <c r="M34" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>17.238582677165354</v>
       </c>
       <c r="N34" s="6" t="s">
@@ -1507,60 +1558,67 @@
         <v>68</v>
       </c>
       <c r="T34" s="8">
-        <f>L34*M34</f>
+        <f t="shared" si="0"/>
         <v>478.07883501766997</v>
       </c>
       <c r="U34" s="10">
         <v>16.86</v>
       </c>
-      <c r="V34" s="10">
-        <f>T34/$T$43*$T$24</f>
+      <c r="V34" s="1">
+        <v>37</v>
+      </c>
+      <c r="W34" s="10">
+        <f t="shared" si="1"/>
         <v>29.825803985557346</v>
       </c>
-      <c r="W34" s="10">
-        <f>T34*$T$21</f>
+      <c r="X34" s="10">
+        <f t="shared" si="2"/>
         <v>10.7069739092499</v>
       </c>
-      <c r="X34" s="10">
-        <f>U34-W34</f>
+      <c r="Y34" s="10">
+        <f t="shared" si="3"/>
         <v>6.1530260907500995</v>
       </c>
-      <c r="Y34" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z34" s="10">
+        <f t="shared" si="8"/>
         <v>6.8410049508462259E-2</v>
       </c>
-      <c r="Z34" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA34" s="10">
+        <f t="shared" si="9"/>
         <v>6.1530260907500995</v>
       </c>
-      <c r="AA34" s="8">
+      <c r="AB34" s="8">
         <v>3</v>
       </c>
-      <c r="AB34" s="10">
-        <f>X34/AA34</f>
+      <c r="AC34" s="10">
+        <f t="shared" si="4"/>
         <v>2.0510086969166998</v>
       </c>
-      <c r="AC34" s="10">
-        <f>AA34*$AB$43</f>
+      <c r="AD34" s="10">
+        <f t="shared" si="5"/>
         <v>1.2254944243482235</v>
       </c>
-      <c r="AD34" s="10">
-        <f>X34-AC34</f>
+      <c r="AE34" s="10">
+        <f t="shared" si="6"/>
         <v>4.927531666401876</v>
       </c>
-      <c r="AE34" s="8">
+      <c r="AF34" s="10">
+        <f t="shared" si="10"/>
+        <v>4.2126943350787781E-2</v>
+      </c>
+      <c r="AG34" s="8">
         <v>2</v>
       </c>
-      <c r="AF34" s="10">
-        <f t="shared" si="4"/>
+      <c r="AH34" s="10">
+        <f t="shared" si="12"/>
         <v>16.86</v>
       </c>
-      <c r="AG34" s="14">
-        <f t="shared" si="3"/>
-        <v>7.268650203726118E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI34" s="15">
+        <f t="shared" si="11"/>
+        <v>239.03941750883499</v>
+      </c>
+    </row>
+    <row r="35" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C35" s="4">
         <v>6</v>
       </c>
@@ -1589,11 +1647,11 @@
         <v>323.14</v>
       </c>
       <c r="L35" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>12.722047244094489</v>
       </c>
       <c r="M35" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>12.722047244094489</v>
       </c>
       <c r="N35" s="6" t="s">
@@ -1609,60 +1667,64 @@
         <v>71</v>
       </c>
       <c r="T35" s="8">
-        <f>L35*M35</f>
+        <f t="shared" si="0"/>
         <v>161.85048608097216</v>
       </c>
       <c r="U35" s="10">
         <v>38.57</v>
       </c>
-      <c r="V35" s="10">
-        <f>T35/$T$43*$T$24</f>
+      <c r="V35" s="1">
+        <v>23</v>
+      </c>
+      <c r="W35" s="10">
+        <f t="shared" si="1"/>
         <v>10.097332321017378</v>
       </c>
-      <c r="W35" s="10">
-        <f>T35*$T$21</f>
+      <c r="X35" s="10">
+        <f t="shared" si="2"/>
         <v>3.6247765111884389</v>
       </c>
-      <c r="X35" s="10">
-        <f>U35-W35</f>
+      <c r="Y35" s="10">
+        <f t="shared" si="3"/>
         <v>34.945223488811564</v>
       </c>
-      <c r="Y35" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z35" s="10">
+        <f t="shared" si="8"/>
         <v>0.68670597621449969</v>
       </c>
-      <c r="Z35" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA35" s="10">
+        <f t="shared" si="9"/>
         <v>3.481263527269999</v>
       </c>
-      <c r="AA35" s="8">
+      <c r="AB35" s="8">
         <v>8</v>
       </c>
-      <c r="AB35" s="10">
-        <f>X35/AA35</f>
+      <c r="AC35" s="10">
+        <f t="shared" si="4"/>
         <v>4.3681529361014455</v>
       </c>
-      <c r="AC35" s="10">
-        <f>AA35*$AB$43</f>
+      <c r="AD35" s="10">
+        <f t="shared" si="5"/>
         <v>3.267985131595263</v>
       </c>
-      <c r="AD35" s="10">
-        <f>X35-AC35</f>
+      <c r="AE35" s="10">
+        <f t="shared" si="6"/>
         <v>31.6772383572163</v>
       </c>
-      <c r="AE35" s="8">
+      <c r="AF35" s="10"/>
+      <c r="AG35" s="8">
         <v>2</v>
       </c>
-      <c r="AF35" s="10">
-        <f>MIN(U35:V35)</f>
+      <c r="AH35" s="10">
+        <f>MIN(U35:W35)</f>
         <v>10.097332321017378</v>
       </c>
-      <c r="AG35" s="14">
-        <f t="shared" si="3"/>
-        <v>8.4728678547971559E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="3:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI35" s="15">
+        <f t="shared" si="11"/>
+        <v>80.92524304048608</v>
+      </c>
+    </row>
+    <row r="36" spans="3:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="4">
         <v>7</v>
       </c>
@@ -1691,11 +1753,11 @@
         <v>295.10000000000002</v>
       </c>
       <c r="L36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>9.8818897637795278</v>
       </c>
       <c r="M36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>11.618110236220474</v>
       </c>
       <c r="N36" s="6" t="s">
@@ -1714,60 +1776,64 @@
         <v>66</v>
       </c>
       <c r="T36" s="8">
-        <f>L36*M36</f>
+        <f t="shared" si="0"/>
         <v>114.80888461776925</v>
       </c>
       <c r="U36" s="10">
         <v>6.13</v>
       </c>
-      <c r="V36" s="10">
-        <f>T36/$T$43*$T$24</f>
+      <c r="V36" s="1">
+        <v>12</v>
+      </c>
+      <c r="W36" s="10">
+        <f t="shared" si="1"/>
         <v>7.1625577992455849</v>
       </c>
-      <c r="W36" s="10">
-        <f>T36*$T$21</f>
+      <c r="X36" s="10">
+        <f t="shared" si="2"/>
         <v>2.571240645085457</v>
       </c>
-      <c r="X36" s="10">
-        <f>U36-W36</f>
+      <c r="Y36" s="10">
+        <f t="shared" si="3"/>
         <v>3.5587593549145429</v>
       </c>
-      <c r="Y36" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z36" s="10">
+        <f t="shared" si="8"/>
         <v>8.2761845463128911E-2</v>
       </c>
-      <c r="Z36" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA36" s="10">
+        <f t="shared" si="9"/>
         <v>2.9416321288638771</v>
       </c>
-      <c r="AA36" s="8">
+      <c r="AB36" s="8">
         <v>6</v>
       </c>
-      <c r="AB36" s="10">
-        <f>X36/AA36</f>
+      <c r="AC36" s="10">
+        <f t="shared" si="4"/>
         <v>0.59312655915242385</v>
       </c>
-      <c r="AC36" s="10">
-        <f>AA36*$AB$43</f>
+      <c r="AD36" s="10">
+        <f t="shared" si="5"/>
         <v>2.4509888486964471</v>
       </c>
-      <c r="AD36" s="10">
-        <f>X36-AC36</f>
+      <c r="AE36" s="10">
+        <f t="shared" si="6"/>
         <v>1.1077705062180958</v>
       </c>
-      <c r="AE36" s="8">
+      <c r="AF36" s="10"/>
+      <c r="AG36" s="8">
         <v>1</v>
       </c>
-      <c r="AF36" s="10">
-        <f t="shared" si="4"/>
+      <c r="AH36" s="10">
+        <f t="shared" si="12"/>
         <v>6.13</v>
       </c>
-      <c r="AG36" s="14">
-        <f t="shared" si="3"/>
-        <v>0.39983504872698972</v>
-      </c>
-    </row>
-    <row r="37" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI36" s="15">
+        <f t="shared" si="11"/>
+        <v>57.404442308884626</v>
+      </c>
+    </row>
+    <row r="37" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C37" s="4">
         <v>8</v>
       </c>
@@ -1796,11 +1862,11 @@
         <v>269.48</v>
       </c>
       <c r="L37" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>13.779527559055119</v>
       </c>
       <c r="M37" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>10.60944881889764</v>
       </c>
       <c r="N37" s="6" t="s">
@@ -1819,60 +1885,64 @@
         <v>67</v>
       </c>
       <c r="T37" s="8">
-        <f>L37*M37</f>
+        <f t="shared" si="0"/>
         <v>146.19319238638479</v>
       </c>
       <c r="U37" s="10">
         <v>12.37</v>
       </c>
-      <c r="V37" s="10">
-        <f>T37/$T$43*$T$24</f>
+      <c r="V37" s="1">
+        <v>30</v>
+      </c>
+      <c r="W37" s="10">
+        <f t="shared" si="1"/>
         <v>9.1205240239886969</v>
       </c>
-      <c r="W37" s="10">
-        <f>T37*$T$21</f>
+      <c r="X37" s="10">
+        <f t="shared" si="2"/>
         <v>3.2741183711534094</v>
       </c>
-      <c r="X37" s="10">
-        <f>U37-W37</f>
+      <c r="Y37" s="10">
+        <f t="shared" si="3"/>
         <v>9.0958816288465894</v>
       </c>
-      <c r="Y37" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z37" s="10">
+        <f t="shared" si="8"/>
         <v>0.18647526423185845</v>
       </c>
-      <c r="Z37" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA37" s="10">
+        <f t="shared" si="9"/>
         <v>3.3369021629529296</v>
       </c>
-      <c r="AA37" s="8">
+      <c r="AB37" s="8">
         <v>13</v>
       </c>
-      <c r="AB37" s="10">
-        <f>X37/AA37</f>
+      <c r="AC37" s="10">
+        <f t="shared" si="4"/>
         <v>0.6996832022189684</v>
       </c>
-      <c r="AC37" s="10">
-        <f>AA37*$AB$43</f>
+      <c r="AD37" s="10">
+        <f t="shared" si="5"/>
         <v>5.3104758388423026</v>
       </c>
-      <c r="AD37" s="10">
-        <f>X37-AC37</f>
+      <c r="AE37" s="10">
+        <f t="shared" si="6"/>
         <v>3.7854057900042868</v>
       </c>
-      <c r="AE37" s="8">
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="8">
         <v>1</v>
       </c>
-      <c r="AF37" s="10">
-        <f t="shared" si="4"/>
+      <c r="AH37" s="10">
+        <f t="shared" si="12"/>
         <v>12.37</v>
       </c>
-      <c r="AG37" s="14">
-        <f t="shared" si="3"/>
-        <v>0.42930281639792262</v>
-      </c>
-    </row>
-    <row r="38" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI37" s="15">
+        <f t="shared" si="11"/>
+        <v>73.096596193192397</v>
+      </c>
+    </row>
+    <row r="38" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C38" s="4">
         <v>9</v>
       </c>
@@ -1901,11 +1971,11 @@
         <v>208.01</v>
       </c>
       <c r="L38" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>47.309448818897643</v>
       </c>
       <c r="M38" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8.1893700787401578</v>
       </c>
       <c r="N38" s="6" t="s">
@@ -1924,57 +1994,61 @@
         <v>67</v>
       </c>
       <c r="T38" s="8">
-        <f>L38*M38</f>
+        <f t="shared" si="0"/>
         <v>387.43458459916923</v>
       </c>
       <c r="U38" s="10">
         <v>21.55</v>
       </c>
-      <c r="V38" s="10">
-        <f>T38/$T$43*$T$24</f>
+      <c r="V38" s="1">
+        <v>19</v>
+      </c>
+      <c r="W38" s="10">
+        <f t="shared" si="1"/>
         <v>24.170800150677156</v>
       </c>
-      <c r="W38" s="10">
-        <f>T38*$T$21</f>
+      <c r="X38" s="10">
+        <f t="shared" si="2"/>
         <v>8.6769203842522273</v>
       </c>
-      <c r="X38" s="10">
-        <f>U38-W38</f>
+      <c r="Y38" s="10">
+        <f t="shared" si="3"/>
         <v>12.873079615747773</v>
       </c>
-      <c r="Y38" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z38" s="10">
+        <f t="shared" si="8"/>
         <v>0.11597615833492711</v>
       </c>
-      <c r="Z38" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA38" s="10">
+        <f t="shared" si="9"/>
         <v>7.5933538968971659</v>
       </c>
-      <c r="AA38" s="8">
+      <c r="AB38" s="8">
         <v>16</v>
       </c>
-      <c r="AB38" s="10">
-        <f>X38/AA38</f>
+      <c r="AC38" s="10">
+        <f t="shared" si="4"/>
         <v>0.80456747598423584</v>
       </c>
-      <c r="AC38" s="10">
-        <f>AA38*$AB$43</f>
+      <c r="AD38" s="10">
+        <f t="shared" si="5"/>
         <v>6.5359702631905261</v>
       </c>
-      <c r="AD38" s="10">
-        <f>X38-AC38</f>
+      <c r="AE38" s="10">
+        <f t="shared" si="6"/>
         <v>6.3371093525572473</v>
       </c>
-      <c r="AE38" s="8">
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="8">
         <v>0</v>
       </c>
-      <c r="AF38" s="10"/>
-      <c r="AG38" s="14">
-        <f t="shared" si="3"/>
-        <v>0.3032932836747344</v>
-      </c>
-    </row>
-    <row r="39" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AH38" s="10"/>
+      <c r="AI38" s="15">
+        <f t="shared" si="11"/>
+        <v>193.71729229958461</v>
+      </c>
+    </row>
+    <row r="39" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C39" s="4">
         <v>10</v>
       </c>
@@ -2003,11 +2077,11 @@
         <v>211.01</v>
       </c>
       <c r="L39" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>38.648031496062991</v>
       </c>
       <c r="M39" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8.30748031496063</v>
       </c>
       <c r="N39" s="6" t="s">
@@ -2026,57 +2100,61 @@
         <v>67</v>
       </c>
       <c r="T39" s="8">
-        <f>L39*M39</f>
+        <f t="shared" si="0"/>
         <v>321.06776086552173</v>
       </c>
       <c r="U39" s="10">
         <v>22.24</v>
       </c>
-      <c r="V39" s="10">
-        <f>T39/$T$43*$T$24</f>
+      <c r="V39" s="1">
+        <v>26</v>
+      </c>
+      <c r="W39" s="10">
+        <f t="shared" si="1"/>
         <v>20.030387041298145</v>
       </c>
-      <c r="W39" s="10">
-        <f>T39*$T$21</f>
+      <c r="X39" s="10">
+        <f t="shared" si="2"/>
         <v>7.1905800610507473</v>
       </c>
-      <c r="X39" s="10">
-        <f>U39-W39</f>
+      <c r="Y39" s="10">
+        <f t="shared" si="3"/>
         <v>15.049419938949251</v>
       </c>
-      <c r="Y39" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z39" s="10">
+        <f t="shared" si="8"/>
         <v>0.16025189970792886</v>
       </c>
-      <c r="Z39" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA39" s="10">
+        <f t="shared" si="9"/>
         <v>6.4244577753746199</v>
       </c>
-      <c r="AA39" s="8">
+      <c r="AB39" s="8">
         <v>18</v>
       </c>
-      <c r="AB39" s="10">
-        <f>X39/AA39</f>
+      <c r="AC39" s="10">
+        <f t="shared" si="4"/>
         <v>0.83607888549718057</v>
       </c>
-      <c r="AC39" s="10">
-        <f>AA39*$AB$43</f>
+      <c r="AD39" s="10">
+        <f t="shared" si="5"/>
         <v>7.3529665460893421</v>
       </c>
-      <c r="AD39" s="10">
-        <f>X39-AC39</f>
+      <c r="AE39" s="10">
+        <f t="shared" si="6"/>
         <v>7.696453392859909</v>
       </c>
-      <c r="AE39" s="8">
+      <c r="AF39" s="10"/>
+      <c r="AG39" s="8">
         <v>0</v>
       </c>
-      <c r="AF39" s="10"/>
-      <c r="AG39" s="14">
-        <f t="shared" si="3"/>
-        <v>0.33061899937452083</v>
-      </c>
-    </row>
-    <row r="40" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AH39" s="10"/>
+      <c r="AI39" s="15">
+        <f t="shared" si="11"/>
+        <v>160.53388043276087</v>
+      </c>
+    </row>
+    <row r="40" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C40" s="4">
         <v>11</v>
       </c>
@@ -2102,11 +2180,11 @@
         <v>216.31</v>
       </c>
       <c r="L40" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>13.062204724409449</v>
       </c>
       <c r="M40" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8.5161417322834652</v>
       </c>
       <c r="N40" s="6" t="s">
@@ -2125,60 +2203,64 @@
         <v>66</v>
       </c>
       <c r="T40" s="8">
-        <f>L40*M40</f>
+        <f t="shared" si="0"/>
         <v>111.23958676917356</v>
       </c>
       <c r="U40" s="10">
         <v>6.55</v>
       </c>
-      <c r="V40" s="10">
-        <f>T40/$T$43*$T$24</f>
+      <c r="V40" s="1">
+        <v>9</v>
+      </c>
+      <c r="W40" s="10">
+        <f t="shared" si="1"/>
         <v>6.9398807631572756</v>
       </c>
-      <c r="W40" s="10">
-        <f>T40*$T$21</f>
+      <c r="X40" s="10">
+        <f t="shared" si="2"/>
         <v>2.4913032453512827</v>
       </c>
-      <c r="X40" s="10">
-        <f>U40-W40</f>
+      <c r="Y40" s="10">
+        <f t="shared" si="3"/>
         <v>4.0586967546487172</v>
       </c>
-      <c r="Y40" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z40" s="10">
+        <f t="shared" si="8"/>
         <v>9.4045592483056994E-2</v>
       </c>
-      <c r="Z40" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA40" s="10">
+        <f t="shared" si="9"/>
         <v>2.9523514988262267</v>
       </c>
-      <c r="AA40" s="8">
+      <c r="AB40" s="8">
         <v>7</v>
       </c>
-      <c r="AB40" s="10">
-        <f>X40/AA40</f>
+      <c r="AC40" s="10">
+        <f t="shared" si="4"/>
         <v>0.57981382209267385</v>
       </c>
-      <c r="AC40" s="10">
-        <f>AA40*$AB$43</f>
+      <c r="AD40" s="10">
+        <f t="shared" si="5"/>
         <v>2.8594869901458551</v>
       </c>
-      <c r="AD40" s="10">
-        <f>X40-AC40</f>
+      <c r="AE40" s="10">
+        <f t="shared" si="6"/>
         <v>1.1992097645028621</v>
       </c>
-      <c r="AE40" s="8">
+      <c r="AF40" s="10"/>
+      <c r="AG40" s="8">
         <v>1</v>
       </c>
-      <c r="AF40" s="10">
-        <f t="shared" ref="AF40:AF42" si="5">U40</f>
+      <c r="AH40" s="10">
+        <f t="shared" ref="AH40:AH42" si="13">U40</f>
         <v>6.55</v>
       </c>
-      <c r="AG40" s="14">
-        <f t="shared" si="3"/>
-        <v>0.43656289925890918</v>
-      </c>
-    </row>
-    <row r="41" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI40" s="15">
+        <f t="shared" si="11"/>
+        <v>55.619793384586778</v>
+      </c>
+    </row>
+    <row r="41" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C41" s="4">
         <v>12</v>
       </c>
@@ -2204,11 +2286,11 @@
         <v>92.19</v>
       </c>
       <c r="L41" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>1.1811023622047245</v>
       </c>
       <c r="M41" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>3.6295275590551181</v>
       </c>
       <c r="N41" s="6" t="s">
@@ -2227,60 +2309,64 @@
         <v>69</v>
       </c>
       <c r="T41" s="8">
-        <f>L41*M41</f>
+        <f t="shared" si="0"/>
         <v>4.2868435736871477</v>
       </c>
       <c r="U41" s="10">
         <v>1.73</v>
       </c>
-      <c r="V41" s="10">
-        <f>T41/$T$43*$T$24</f>
+      <c r="V41" s="1">
+        <v>2</v>
+      </c>
+      <c r="W41" s="10">
+        <f t="shared" si="1"/>
         <v>0.26744241070787694</v>
       </c>
-      <c r="W41" s="10">
-        <f>T41*$T$21</f>
+      <c r="X41" s="10">
+        <f t="shared" si="2"/>
         <v>9.6007434202368416E-2</v>
       </c>
-      <c r="X41" s="10">
-        <f>U41-W41</f>
+      <c r="Y41" s="10">
+        <f t="shared" si="3"/>
         <v>1.6339925657976315</v>
       </c>
-      <c r="Y41" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z41" s="10">
+        <f t="shared" si="8"/>
         <v>0.16983145581168607</v>
       </c>
-      <c r="Z41" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA41" s="10">
+        <f t="shared" si="9"/>
         <v>0.65819086216055145</v>
       </c>
-      <c r="AA41" s="8">
+      <c r="AB41" s="8">
         <v>4</v>
       </c>
-      <c r="AB41" s="10">
-        <f>X41/AA41</f>
+      <c r="AC41" s="10">
+        <f t="shared" si="4"/>
         <v>0.40849814144940788</v>
       </c>
-      <c r="AC41" s="10">
-        <f>AA41*$AB$43</f>
+      <c r="AD41" s="10">
+        <f t="shared" si="5"/>
         <v>1.6339925657976315</v>
       </c>
-      <c r="AD41" s="10">
-        <f>X41-AC41</f>
+      <c r="AE41" s="10">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AE41" s="8">
+      <c r="AF41" s="10"/>
+      <c r="AG41" s="8">
         <v>1</v>
       </c>
-      <c r="AF41" s="10">
-        <f t="shared" si="5"/>
+      <c r="AH41" s="10">
+        <f t="shared" si="13"/>
         <v>1.73</v>
       </c>
-      <c r="AG41" s="14">
-        <f t="shared" si="3"/>
-        <v>0.94450437329342862</v>
-      </c>
-    </row>
-    <row r="42" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI41" s="15">
+        <f t="shared" si="11"/>
+        <v>2.1434217868435739</v>
+      </c>
+    </row>
+    <row r="42" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C42" s="4">
         <v>13</v>
       </c>
@@ -2306,11 +2392,11 @@
         <v>118.83</v>
       </c>
       <c r="L42" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>2.598425196850394</v>
       </c>
       <c r="M42" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>4.6783464566929132</v>
       </c>
       <c r="N42" s="6" t="s">
@@ -2329,60 +2415,64 @@
         <v>66</v>
       </c>
       <c r="T42" s="8">
-        <f>L42*M42</f>
+        <f t="shared" si="0"/>
         <v>12.156333312666627</v>
       </c>
       <c r="U42" s="10">
         <v>1.45</v>
       </c>
-      <c r="V42" s="10">
-        <f>T42/$T$43*$T$24</f>
+      <c r="V42" s="1">
+        <v>2</v>
+      </c>
+      <c r="W42" s="10">
+        <f t="shared" si="1"/>
         <v>0.75839461613751413</v>
       </c>
-      <c r="W42" s="10">
-        <f>T42*$T$21</f>
+      <c r="X42" s="10">
+        <f t="shared" si="2"/>
         <v>0.27225121481492964</v>
       </c>
-      <c r="X42" s="10">
-        <f>U42-W42</f>
+      <c r="Y42" s="10">
+        <f t="shared" si="3"/>
         <v>1.1777487851850703</v>
       </c>
-      <c r="Y42" s="10">
-        <f t="shared" si="1"/>
+      <c r="Z42" s="10">
+        <f t="shared" si="8"/>
         <v>8.0925226271981787E-2</v>
       </c>
-      <c r="Z42" s="10">
-        <f t="shared" si="2"/>
+      <c r="AA42" s="10">
+        <f t="shared" si="9"/>
         <v>0.99560861816134483</v>
       </c>
-      <c r="AA42" s="8">
+      <c r="AB42" s="8">
         <v>1</v>
       </c>
-      <c r="AB42" s="10">
-        <f>X42/AA42</f>
+      <c r="AC42" s="10">
+        <f t="shared" si="4"/>
         <v>1.1777487851850703</v>
       </c>
-      <c r="AC42" s="10">
-        <f>AA42*$AB$43</f>
+      <c r="AD42" s="10">
+        <f t="shared" si="5"/>
         <v>0.40849814144940788</v>
       </c>
-      <c r="AD42" s="10">
-        <f>X42-AC42</f>
+      <c r="AE42" s="10">
+        <f t="shared" si="6"/>
         <v>0.76925064373566243</v>
       </c>
-      <c r="AE42" s="8">
+      <c r="AF42" s="10"/>
+      <c r="AG42" s="8">
         <v>1</v>
       </c>
-      <c r="AF42" s="10">
-        <f t="shared" si="5"/>
+      <c r="AH42" s="10">
+        <f t="shared" si="13"/>
         <v>1.45</v>
       </c>
-      <c r="AG42" s="14">
-        <f t="shared" si="3"/>
-        <v>0.28172285617200543</v>
-      </c>
-    </row>
-    <row r="43" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AI42" s="15">
+        <f t="shared" si="11"/>
+        <v>6.0781666563333134</v>
+      </c>
+    </row>
+    <row r="43" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
       <c r="T43" s="10">
         <f>SUMPRODUCT(E30:E42,T30:T42)</f>
@@ -2394,38 +2484,46 @@
       </c>
       <c r="V43" s="10">
         <f>SUMPRODUCT(E30:E42,V30:V42)</f>
+        <v>321</v>
+      </c>
+      <c r="W43" s="10">
+        <f>SUMPRODUCT(E30:E42,W30:W42)</f>
         <v>200.00000000000003</v>
       </c>
-      <c r="W43" s="10">
-        <f>T43*$T$21</f>
+      <c r="X43" s="10">
+        <f t="shared" si="2"/>
         <v>71.796716121614537</v>
       </c>
-      <c r="X43" s="10"/>
-      <c r="Y43" s="10">
-        <f>MIN(Y30:Y42)</f>
+      <c r="Y43" s="10"/>
+      <c r="Z43" s="10">
+        <f>MIN(Z30:Z42)</f>
         <v>6.8410049508462259E-2</v>
       </c>
-      <c r="Z43" s="10">
-        <f>SUMPRODUCT(Z30:Z42,E30:E42)</f>
+      <c r="AA43" s="10">
+        <f>SUMPRODUCT(AA30:AA42,E30:E42)</f>
         <v>62.499582829473269</v>
       </c>
-      <c r="AA43" s="10"/>
-      <c r="AB43" s="10">
-        <f>MIN(AB30:AB42)</f>
+      <c r="AB43" s="10"/>
+      <c r="AC43" s="10">
+        <f>MIN(AC30:AC42)</f>
         <v>0.40849814144940788</v>
       </c>
-      <c r="AC43" s="10">
-        <f>SUMPRODUCT(AC30:AC42,E30:E42)</f>
+      <c r="AD43" s="10">
+        <f>SUMPRODUCT(AD30:AD42,E30:E42)</f>
         <v>51.879263964074795</v>
       </c>
-      <c r="AD43" s="10"/>
       <c r="AE43" s="10"/>
       <c r="AF43" s="10">
-        <f>SUMPRODUCT(AE30:AE42,AF30:AF42)</f>
+        <f>MIN(AF30:AF34)</f>
+        <v>4.2126943350787781E-2</v>
+      </c>
+      <c r="AG43" s="10"/>
+      <c r="AH43" s="10">
+        <f>SUMPRODUCT(AG30:AG42,AH30:AH42)</f>
         <v>123.48466464203476</v>
       </c>
     </row>
-    <row r="44" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>59</v>
       </c>
@@ -2442,8 +2540,10 @@
       <c r="AD44" s="10"/>
       <c r="AE44" s="10"/>
       <c r="AF44" s="10"/>
-    </row>
-    <row r="45" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AG44" s="10"/>
+      <c r="AH44" s="10"/>
+    </row>
+    <row r="45" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C45" s="8">
         <f>SUMPRODUCT(L30:L36,M30:M36,E30:E36)</f>
         <v>2107.9021275342552</v>
@@ -2452,12 +2552,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C47" s="8">
         <f>SUMPRODUCT(M37:M39,L37:L39,E37:E39)</f>
         <v>854.69553785107564</v>
@@ -2466,12 +2566,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T48" s="1"/>
+    </row>
+    <row r="49" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C49" s="8">
         <f>SUMPRODUCT(E40:E42,L40:L42,M40:M42)</f>
         <v>243.20919399838803</v>
@@ -2479,13 +2580,29 @@
       <c r="D49" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T49" s="11"/>
+      <c r="W49" s="10"/>
+    </row>
+    <row r="50" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T50" s="11"/>
+      <c r="W50" s="10"/>
+    </row>
+    <row r="51" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T51" s="11"/>
+      <c r="W51" s="10"/>
+    </row>
+    <row r="52" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T52" s="11"/>
+      <c r="W52" s="10"/>
+    </row>
+    <row r="53" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T53" s="11"/>
+      <c r="W53" s="10"/>
+    </row>
+    <row r="54" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>81</v>
       </c>
@@ -2498,8 +2615,10 @@
       <c r="F54" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T54" s="11"/>
+      <c r="W54" s="10"/>
+    </row>
+    <row r="55" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>1</v>
       </c>
@@ -2512,8 +2631,10 @@
       <c r="F55" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T55" s="11"/>
+      <c r="W55" s="10"/>
+    </row>
+    <row r="56" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>2</v>
       </c>
@@ -2526,8 +2647,10 @@
       <c r="F56" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T56" s="11"/>
+      <c r="W56" s="10"/>
+    </row>
+    <row r="57" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>3</v>
       </c>
@@ -2540,8 +2663,10 @@
       <c r="F57" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T57" s="11"/>
+      <c r="W57" s="10"/>
+    </row>
+    <row r="58" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>4</v>
       </c>
@@ -2554,8 +2679,10 @@
       <c r="F58" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T58" s="11"/>
+      <c r="W58" s="10"/>
+    </row>
+    <row r="59" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>5</v>
       </c>
@@ -2568,8 +2695,10 @@
       <c r="F59" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T59" s="11"/>
+      <c r="W59" s="10"/>
+    </row>
+    <row r="60" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>6</v>
       </c>
@@ -2582,8 +2711,10 @@
       <c r="F60" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T60" s="11"/>
+      <c r="W60" s="10"/>
+    </row>
+    <row r="61" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>7</v>
       </c>
@@ -2593,8 +2724,10 @@
       <c r="E61">
         <v>0.40600000000000003</v>
       </c>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T61" s="11"/>
+      <c r="W61" s="10"/>
+    </row>
+    <row r="62" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
         <v>8</v>
       </c>
@@ -2604,8 +2737,10 @@
       <c r="E62">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="T62" s="1"/>
+      <c r="W62" s="10"/>
+    </row>
+    <row r="63" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
         <v>9</v>
       </c>
@@ -2616,7 +2751,7 @@
         <v>0.94499999999999995</v>
       </c>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
         <v>10</v>
       </c>

</xml_diff>